<commit_message>
Updated as of 2/8/18
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a958261cafb92040/DataScience/Capstone/Products/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TMccw\OneDrive\DataScience\Capstone\Products\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>Start Date</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Meeting # 9</t>
   </si>
   <si>
-    <t>Meeting with Advisor # 5</t>
-  </si>
-  <si>
     <t>Meeting # 10</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>Initial Design Plan Submission</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Not Started</t>
   </si>
   <si>
@@ -174,6 +168,9 @@
   </si>
   <si>
     <t xml:space="preserve">Blockchain for Anti-Money Laundering                     </t>
+  </si>
+  <si>
+    <t>Meeting with Advisor # 8</t>
   </si>
 </sst>
 </file>
@@ -281,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,12 +299,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,7 +392,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -452,13 +443,10 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,10 +594,10 @@
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Meeting # 7</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Meeting with Advisor # 2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Meeting # 7</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Meeting with Advisor # 3</c:v>
@@ -624,13 +612,13 @@
                   <c:v>Meeting # 9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Meeting with Advisor # 5</c:v>
+                  <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>Meeting # 10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Meeting with Advisor # 6</c:v>
+                  <c:v>Meeting with Advisor # 7</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>Meeting # 11</c:v>
@@ -645,7 +633,7 @@
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Meeting with Advisor # 7</c:v>
+                  <c:v>Meeting with Advisor # 8</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>Meeting # 13</c:v>
@@ -726,7 +714,7 @@
                   <c:v>43138</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43139</c:v>
+                  <c:v>43141</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>43142</c:v>
@@ -1321,10 +1309,10 @@
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Meeting # 7</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Meeting with Advisor # 2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Meeting # 7</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Meeting with Advisor # 3</c:v>
@@ -1339,13 +1327,13 @@
                   <c:v>Meeting # 9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Meeting with Advisor # 5</c:v>
+                  <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>Meeting # 10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Meeting with Advisor # 6</c:v>
+                  <c:v>Meeting with Advisor # 7</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>Meeting # 11</c:v>
@@ -1360,7 +1348,7 @@
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Meeting with Advisor # 7</c:v>
+                  <c:v>Meeting with Advisor # 8</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>Meeting # 13</c:v>
@@ -2537,7 +2525,9 @@
   </sheetPr>
   <dimension ref="B1:U55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2560,10 +2550,10 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -2571,10 +2561,10 @@
     </row>
     <row r="2" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -2606,7 +2596,7 @@
         <v>43332</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
@@ -2634,19 +2624,19 @@
       <c r="U6" s="4"/>
     </row>
     <row r="7" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="4"/>
@@ -2657,14 +2647,14 @@
         <f>C8</f>
         <v>43118</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
     </row>
     <row r="8" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
@@ -2681,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -2700,7 +2690,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -2719,7 +2709,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -2738,7 +2728,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -2757,7 +2747,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -2776,7 +2766,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -2794,8 +2784,8 @@
         <f t="shared" ref="E14" si="1">IF(ISBLANK(C14),"", (D14-C14+1))</f>
         <v>8</v>
       </c>
-      <c r="F14" s="22" t="s">
-        <v>45</v>
+      <c r="F14" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -2814,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G15" s="4"/>
     </row>
@@ -2833,13 +2823,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="18">
         <v>43131</v>
@@ -2851,8 +2841,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="F17" s="22" t="s">
-        <v>45</v>
+      <c r="F17" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G17" s="4"/>
     </row>
@@ -2870,8 +2860,8 @@
         <f t="shared" ref="E18:E34" si="3">IF(ISBLANK(C18),"", (D18-C18+1))</f>
         <v>1</v>
       </c>
-      <c r="F18" s="23" t="s">
-        <v>46</v>
+      <c r="F18" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -2889,8 +2879,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F19" s="23" t="s">
-        <v>46</v>
+      <c r="F19" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G19" s="4"/>
     </row>
@@ -2908,14 +2898,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F20" s="23" t="s">
-        <v>46</v>
+      <c r="F20" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="18">
         <v>43138</v>
@@ -2927,33 +2917,33 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="F21" s="23" t="s">
-        <v>46</v>
+      <c r="F21" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C22" s="18">
-        <v>43139</v>
+        <v>43141</v>
       </c>
       <c r="D22" s="18">
-        <v>43139</v>
+        <v>43141</v>
       </c>
       <c r="E22" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F22" s="23" t="s">
-        <v>46</v>
+      <c r="F22" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="18">
         <v>43142</v>
@@ -2965,8 +2955,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F23" s="23" t="s">
-        <v>46</v>
+      <c r="F23" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G23" s="4"/>
     </row>
@@ -2984,8 +2974,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F24" s="23" t="s">
-        <v>46</v>
+      <c r="F24" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G24" s="4"/>
     </row>
@@ -3003,8 +2993,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>46</v>
+      <c r="F25" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G25" s="4"/>
     </row>
@@ -3022,8 +3012,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F26" s="23" t="s">
-        <v>46</v>
+      <c r="F26" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G26" s="4"/>
     </row>
@@ -3041,14 +3031,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F27" s="23" t="s">
-        <v>46</v>
+      <c r="F27" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C28" s="18">
         <v>43160</v>
@@ -3060,14 +3050,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F28" s="23" t="s">
-        <v>46</v>
+      <c r="F28" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="18">
         <v>43163</v>
@@ -3079,14 +3069,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F29" s="23" t="s">
-        <v>46</v>
+      <c r="F29" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C30" s="18">
         <v>43167</v>
@@ -3098,14 +3088,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F30" s="23" t="s">
-        <v>46</v>
+      <c r="F30" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="18">
         <v>43170</v>
@@ -3117,13 +3107,13 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F31" s="23" t="s">
-        <v>46</v>
+      <c r="F31" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="18">
         <v>43172</v>
@@ -3135,13 +3125,13 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F32" s="23" t="s">
-        <v>46</v>
+      <c r="F32" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="18">
         <v>43167</v>
@@ -3153,8 +3143,8 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="F33" s="23" t="s">
-        <v>46</v>
+      <c r="F33" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -3171,13 +3161,13 @@
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="F34" s="23" t="s">
-        <v>46</v>
+      <c r="F34" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35" s="18">
         <v>43179</v>
@@ -3189,24 +3179,24 @@
         <f t="shared" ref="E35:E36" si="4">IF(ISBLANK(C35),"", (D35-C35+1))</f>
         <v>1</v>
       </c>
-      <c r="F35" s="23" t="s">
-        <v>46</v>
+      <c r="F35" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="H35" s="6"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="26"/>
       <c r="R35" s="7"/>
     </row>
     <row r="36" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36" s="18">
         <v>43179</v>
@@ -3218,24 +3208,24 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F36" s="23" t="s">
-        <v>46</v>
+      <c r="F36" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="H36" s="7"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="26"/>
-      <c r="Q36" s="26"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="25"/>
       <c r="R36" s="7"/>
     </row>
     <row r="37" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="18">
         <v>43180</v>
@@ -3247,13 +3237,13 @@
         <f t="shared" ref="E37:E44" si="5">IF(ISBLANK(C37),"", (D37-C37+1))</f>
         <v>2</v>
       </c>
-      <c r="F37" s="23" t="s">
-        <v>46</v>
+      <c r="F37" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -3261,8 +3251,8 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F38" s="23" t="s">
-        <v>46</v>
+      <c r="F38" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3275,8 +3265,8 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F39" s="23" t="s">
-        <v>46</v>
+      <c r="F39" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3289,8 +3279,8 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F40" s="23" t="s">
-        <v>46</v>
+      <c r="F40" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3303,8 +3293,8 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F41" s="23" t="s">
-        <v>46</v>
+      <c r="F41" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3317,8 +3307,8 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F42" s="23" t="s">
-        <v>46</v>
+      <c r="F42" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3331,8 +3321,8 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F43" s="23" t="s">
-        <v>46</v>
+      <c r="F43" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3345,8 +3335,8 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F44" s="23" t="s">
-        <v>46</v>
+      <c r="F44" s="22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Up to date as of 2/17
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan Freeman\Documents\Southern Methodist University - MS in Data Science\Courses\Spring 2018\MSDS 6120 Capstone A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TMccw\OneDrive\DataScience\Capstone\Products\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -162,9 +161,6 @@
     <t>Not Started</t>
   </si>
   <si>
-    <t>Meeting with Advisor # 7</t>
-  </si>
-  <si>
     <t>Meeting # 13</t>
   </si>
   <si>
@@ -172,12 +168,15 @@
   </si>
   <si>
     <t>Meeting with Advisor # 5</t>
+  </si>
+  <si>
+    <t>Meeting # 14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -595,49 +594,49 @@
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Meeting with Advisor # 2</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Meeting # 7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Meeting with Advisor # 2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Meeting # 8</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Meeting # 9</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>Meeting # 9</c:v>
-                </c:pt>
                 <c:pt idx="19">
+                  <c:v>Meeting # 10</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>Meeting with Advisor # 4</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>Meeting # 10</c:v>
-                </c:pt>
                 <c:pt idx="21">
+                  <c:v>Meeting # 11</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>Meeting # 11</c:v>
-                </c:pt>
                 <c:pt idx="23">
+                  <c:v>Meeting # 12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Meeting # 13</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>First Paper Draft Review with Advisor</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Meeting with Advisor # 6</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Meeting # 12</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Meeting with Advisor # 7</c:v>
+                  <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Meeting # 13</c:v>
+                  <c:v>Meeting # 14</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>Online Café Talk</c:v>
@@ -715,40 +714,40 @@
                   <c:v>43138</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43141</c:v>
+                  <c:v>43144</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43144</c:v>
+                  <c:v>43148</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43148</c:v>
+                  <c:v>43153</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43151</c:v>
+                  <c:v>43156</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43155</c:v>
+                  <c:v>43158</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43158</c:v>
+                  <c:v>43162</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43162</c:v>
+                  <c:v>43165</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43165</c:v>
+                  <c:v>43167</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>43169</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43167</c:v>
+                  <c:v>43170</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>43172</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43176</c:v>
+                  <c:v>43172</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>43132</c:v>
@@ -1310,49 +1309,49 @@
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Meeting with Advisor # 2</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Meeting # 7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Meeting with Advisor # 2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Meeting # 8</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Meeting # 9</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>Meeting # 9</c:v>
-                </c:pt>
                 <c:pt idx="19">
+                  <c:v>Meeting # 10</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>Meeting with Advisor # 4</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>Meeting # 10</c:v>
-                </c:pt>
                 <c:pt idx="21">
+                  <c:v>Meeting # 11</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>Meeting # 11</c:v>
-                </c:pt>
                 <c:pt idx="23">
+                  <c:v>Meeting # 12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Meeting # 13</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>First Paper Draft Review with Advisor</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Meeting with Advisor # 6</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Meeting # 12</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Meeting with Advisor # 7</c:v>
+                  <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Meeting # 13</c:v>
+                  <c:v>Meeting # 14</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>Online Café Talk</c:v>
@@ -1457,7 +1456,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>1</c:v>
@@ -2520,13 +2519,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:U55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2552,7 +2553,7 @@
         <v>38</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -2916,46 +2917,46 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="F21" s="22" t="s">
-        <v>44</v>
+      <c r="F21" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="18">
-        <v>43141</v>
+        <v>43144</v>
       </c>
       <c r="D22" s="18">
-        <v>43141</v>
+        <v>43144</v>
       </c>
       <c r="E22" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F22" s="22" t="s">
-        <v>44</v>
+      <c r="F22" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C23" s="18">
-        <v>43144</v>
+        <v>43148</v>
       </c>
       <c r="D23" s="18">
-        <v>43144</v>
+        <v>43148</v>
       </c>
       <c r="E23" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F23" s="22" t="s">
-        <v>44</v>
+      <c r="F23" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G23" s="4"/>
     </row>
@@ -2964,13 +2965,13 @@
         <v>28</v>
       </c>
       <c r="C24" s="18">
-        <v>43148</v>
+        <v>43153</v>
       </c>
       <c r="D24" s="18">
-        <v>43148</v>
+        <v>43153</v>
       </c>
       <c r="E24" s="21">
-        <f>IF(ISBLANK(C24),"", (D24-C24+1))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F24" s="22" t="s">
@@ -2980,13 +2981,13 @@
     </row>
     <row r="25" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C25" s="18">
-        <v>43151</v>
+        <v>43156</v>
       </c>
       <c r="D25" s="18">
-        <v>43151</v>
+        <v>43156</v>
       </c>
       <c r="E25" s="21">
         <f t="shared" si="3"/>
@@ -2999,16 +3000,16 @@
     </row>
     <row r="26" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C26" s="18">
-        <v>43155</v>
+        <v>43158</v>
       </c>
       <c r="D26" s="18">
-        <v>43155</v>
+        <v>43158</v>
       </c>
       <c r="E26" s="21">
-        <f>IF(ISBLANK(C26),"", (D26-C26+1))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F26" s="22" t="s">
@@ -3018,13 +3019,13 @@
     </row>
     <row r="27" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C27" s="18">
-        <v>43158</v>
+        <v>43162</v>
       </c>
       <c r="D27" s="18">
-        <v>43158</v>
+        <v>43162</v>
       </c>
       <c r="E27" s="21">
         <f t="shared" si="3"/>
@@ -3037,16 +3038,16 @@
     </row>
     <row r="28" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" s="18">
-        <v>43162</v>
+        <v>43165</v>
       </c>
       <c r="D28" s="18">
-        <v>43162</v>
+        <v>43165</v>
       </c>
       <c r="E28" s="21">
-        <f>IF(ISBLANK(C28),"", (D28-C28+1))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F28" s="22" t="s">
@@ -3056,13 +3057,13 @@
     </row>
     <row r="29" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C29" s="18">
-        <v>43165</v>
+        <v>43167</v>
       </c>
       <c r="D29" s="18">
-        <v>43165</v>
+        <v>43167</v>
       </c>
       <c r="E29" s="21">
         <f t="shared" si="3"/>
@@ -3075,7 +3076,7 @@
     </row>
     <row r="30" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C30" s="18">
         <v>43169</v>
@@ -3084,7 +3085,7 @@
         <v>43169</v>
       </c>
       <c r="E30" s="21">
-        <f>IF(ISBLANK(C30),"", (D30-C30+1))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F30" s="22" t="s">
@@ -3094,17 +3095,17 @@
     </row>
     <row r="31" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" s="18">
-        <v>43167</v>
+        <v>43170</v>
       </c>
       <c r="D31" s="18">
-        <v>43172</v>
+        <v>43170</v>
       </c>
       <c r="E31" s="21">
-        <f>IF(ISBLANK(C31),"", (D31-C31+1))</f>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="F31" s="22" t="s">
         <v>44</v>
@@ -3112,7 +3113,7 @@
     </row>
     <row r="32" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C32" s="18">
         <v>43172</v>
@@ -3130,13 +3131,13 @@
     </row>
     <row r="33" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C33" s="18">
-        <v>43176</v>
+        <v>43172</v>
       </c>
       <c r="D33" s="18">
-        <v>43176</v>
+        <v>43172</v>
       </c>
       <c r="E33" s="21">
         <f t="shared" si="3"/>
@@ -3166,7 +3167,7 @@
     </row>
     <row r="35" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C35" s="18">
         <v>43179</v>
@@ -3195,7 +3196,7 @@
     </row>
     <row r="36" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C36" s="18">
         <v>43179</v>

</xml_diff>

<commit_message>
Updated through February 21, 2018
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TMccw\OneDrive\DataScience\Capstone\Products\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan Freeman\Documents\Southern Methodist University - MS in Data Science\Courses\Spring 2018\MSDS 6120 Capstone A\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>Start Date</t>
   </si>
@@ -171,12 +171,18 @@
   </si>
   <si>
     <t>Meeting # 14</t>
+  </si>
+  <si>
+    <t>Meeting with Dr. Engels #1</t>
+  </si>
+  <si>
+    <t>Meeting # 15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -548,9 +554,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$44</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$46</c:f>
               <c:strCache>
-                <c:ptCount val="37"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -594,10 +600,10 @@
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Meeting # 7</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Meeting with Advisor # 2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Meeting # 7</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Meeting # 8</c:v>
@@ -606,60 +612,66 @@
                   <c:v>Meeting # 9</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Meeting # 10</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>Meeting # 10</c:v>
-                </c:pt>
                 <c:pt idx="20">
+                  <c:v>Meeting # 11</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>Meeting with Advisor # 4</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Meeting # 11</c:v>
-                </c:pt>
                 <c:pt idx="22">
-                  <c:v>Meeting with Advisor # 5</c:v>
+                  <c:v>Meeting with Dr. Engels #1</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>Meeting # 12</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>Meeting with Advisor # 5</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
+                  <c:v>Meeting # 14</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>First Paper Draft Review with Advisor</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>Meeting # 14</c:v>
-                </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
+                  <c:v>Meeting # 15</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -667,10 +679,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$44</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
                 </c:pt>
@@ -714,51 +726,57 @@
                   <c:v>43138</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>43141</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>43144</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>43148</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>43153</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>43156</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>43158</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>43162</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>43165</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
+                  <c:v>43166</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>43167</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>43169</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>43170</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>43172</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>43172</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>43132</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>43179</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>43179</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>43180</c:v>
                 </c:pt>
               </c:numCache>
@@ -1263,9 +1281,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$44</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$46</c:f>
               <c:strCache>
-                <c:ptCount val="37"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -1309,10 +1327,10 @@
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Meeting # 7</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Meeting with Advisor # 2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Meeting # 7</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Meeting # 8</c:v>
@@ -1321,60 +1339,66 @@
                   <c:v>Meeting # 9</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Meeting # 10</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>Meeting # 10</c:v>
-                </c:pt>
                 <c:pt idx="20">
+                  <c:v>Meeting # 11</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>Meeting with Advisor # 4</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Meeting # 11</c:v>
-                </c:pt>
                 <c:pt idx="22">
-                  <c:v>Meeting with Advisor # 5</c:v>
+                  <c:v>Meeting with Dr. Engels #1</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>Meeting # 12</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>Meeting with Advisor # 5</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
+                  <c:v>Meeting # 14</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>First Paper Draft Review with Advisor</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>Meeting # 14</c:v>
-                </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
+                  <c:v>Meeting # 15</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1382,10 +1406,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$44</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$46</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1465,22 +1489,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
@@ -1495,6 +1519,12 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2519,14 +2549,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:U55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2857,7 +2887,7 @@
         <v>43132</v>
       </c>
       <c r="E18" s="21">
-        <f t="shared" ref="E18:E34" si="3">IF(ISBLANK(C18),"", (D18-C18+1))</f>
+        <f t="shared" ref="E18:E36" si="3">IF(ISBLANK(C18),"", (D18-C18+1))</f>
         <v>1</v>
       </c>
       <c r="F18" s="20" t="s">
@@ -2924,16 +2954,16 @@
     </row>
     <row r="22" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C22" s="18">
-        <v>43144</v>
+        <v>43141</v>
       </c>
       <c r="D22" s="18">
-        <v>43144</v>
+        <v>43141</v>
       </c>
       <c r="E22" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E22" si="4">IF(ISBLANK(C22),"", (D22-C22+1))</f>
         <v>1</v>
       </c>
       <c r="F22" s="20" t="s">
@@ -2943,13 +2973,13 @@
     </row>
     <row r="23" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="18">
-        <v>43148</v>
+        <v>43144</v>
       </c>
       <c r="D23" s="18">
-        <v>43148</v>
+        <v>43144</v>
       </c>
       <c r="E23" s="21">
         <f t="shared" si="3"/>
@@ -2965,17 +2995,17 @@
         <v>28</v>
       </c>
       <c r="C24" s="18">
-        <v>43153</v>
+        <v>43148</v>
       </c>
       <c r="D24" s="18">
-        <v>43153</v>
+        <v>43148</v>
       </c>
       <c r="E24" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F24" s="22" t="s">
-        <v>44</v>
+      <c r="F24" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G24" s="4"/>
     </row>
@@ -2984,10 +3014,10 @@
         <v>30</v>
       </c>
       <c r="C25" s="18">
-        <v>43156</v>
+        <v>43153</v>
       </c>
       <c r="D25" s="18">
-        <v>43156</v>
+        <v>43153</v>
       </c>
       <c r="E25" s="21">
         <f t="shared" si="3"/>
@@ -3000,13 +3030,13 @@
     </row>
     <row r="26" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C26" s="18">
-        <v>43158</v>
+        <v>43156</v>
       </c>
       <c r="D26" s="18">
-        <v>43158</v>
+        <v>43156</v>
       </c>
       <c r="E26" s="21">
         <f t="shared" si="3"/>
@@ -3019,13 +3049,13 @@
     </row>
     <row r="27" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C27" s="18">
-        <v>43162</v>
+        <v>43158</v>
       </c>
       <c r="D27" s="18">
-        <v>43162</v>
+        <v>43158</v>
       </c>
       <c r="E27" s="21">
         <f t="shared" si="3"/>
@@ -3038,13 +3068,13 @@
     </row>
     <row r="28" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C28" s="18">
-        <v>43165</v>
+        <v>43162</v>
       </c>
       <c r="D28" s="18">
-        <v>43165</v>
+        <v>43162</v>
       </c>
       <c r="E28" s="21">
         <f t="shared" si="3"/>
@@ -3057,13 +3087,13 @@
     </row>
     <row r="29" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C29" s="18">
-        <v>43167</v>
+        <v>43165</v>
       </c>
       <c r="D29" s="18">
-        <v>43167</v>
+        <v>43165</v>
       </c>
       <c r="E29" s="21">
         <f t="shared" si="3"/>
@@ -3076,13 +3106,13 @@
     </row>
     <row r="30" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C30" s="18">
-        <v>43169</v>
+        <v>43166</v>
       </c>
       <c r="D30" s="18">
-        <v>43169</v>
+        <v>43166</v>
       </c>
       <c r="E30" s="21">
         <f t="shared" si="3"/>
@@ -3098,10 +3128,10 @@
         <v>34</v>
       </c>
       <c r="C31" s="18">
-        <v>43170</v>
+        <v>43167</v>
       </c>
       <c r="D31" s="18">
-        <v>43170</v>
+        <v>43167</v>
       </c>
       <c r="E31" s="21">
         <f t="shared" si="3"/>
@@ -3113,13 +3143,13 @@
     </row>
     <row r="32" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C32" s="18">
-        <v>43172</v>
+        <v>43169</v>
       </c>
       <c r="D32" s="18">
-        <v>43172</v>
+        <v>43169</v>
       </c>
       <c r="E32" s="21">
         <f t="shared" si="3"/>
@@ -3131,13 +3161,13 @@
     </row>
     <row r="33" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C33" s="18">
-        <v>43172</v>
+        <v>43170</v>
       </c>
       <c r="D33" s="18">
-        <v>43172</v>
+        <v>43170</v>
       </c>
       <c r="E33" s="21">
         <f t="shared" si="3"/>
@@ -3149,17 +3179,17 @@
     </row>
     <row r="34" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C34" s="18">
-        <v>43132</v>
+        <v>43172</v>
       </c>
       <c r="D34" s="18">
-        <v>43173</v>
+        <v>43172</v>
       </c>
       <c r="E34" s="21">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="F34" s="22" t="s">
         <v>44</v>
@@ -3167,16 +3197,16 @@
     </row>
     <row r="35" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C35" s="18">
-        <v>43179</v>
+        <v>43172</v>
       </c>
       <c r="D35" s="18">
-        <v>43179</v>
+        <v>43172</v>
       </c>
       <c r="E35" s="21">
-        <f t="shared" ref="E35:E36" si="4">IF(ISBLANK(C35),"", (D35-C35+1))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F35" s="22" t="s">
@@ -3196,17 +3226,17 @@
     </row>
     <row r="36" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="17" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C36" s="18">
-        <v>43179</v>
+        <v>43132</v>
       </c>
       <c r="D36" s="18">
-        <v>43179</v>
+        <v>43173</v>
       </c>
       <c r="E36" s="21">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>42</v>
       </c>
       <c r="F36" s="22" t="s">
         <v>44</v>
@@ -3225,17 +3255,17 @@
     </row>
     <row r="37" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C37" s="18">
-        <v>43180</v>
+        <v>43179</v>
       </c>
       <c r="D37" s="18">
-        <v>43181</v>
+        <v>43179</v>
       </c>
       <c r="E37" s="21">
-        <f t="shared" ref="E37:E44" si="5">IF(ISBLANK(C37),"", (D37-C37+1))</f>
-        <v>2</v>
+        <f t="shared" ref="E37:E38" si="5">IF(ISBLANK(C37),"", (D37-C37+1))</f>
+        <v>1</v>
       </c>
       <c r="F37" s="22" t="s">
         <v>44</v>
@@ -3243,13 +3273,17 @@
     </row>
     <row r="38" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="21" t="str">
+        <v>50</v>
+      </c>
+      <c r="C38" s="18">
+        <v>43179</v>
+      </c>
+      <c r="D38" s="18">
+        <v>43179</v>
+      </c>
+      <c r="E38" s="21">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="F38" s="22" t="s">
         <v>44</v>
@@ -3257,13 +3291,17 @@
     </row>
     <row r="39" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="21" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>35</v>
+      </c>
+      <c r="C39" s="18">
+        <v>43180</v>
+      </c>
+      <c r="D39" s="18">
+        <v>43181</v>
+      </c>
+      <c r="E39" s="21">
+        <f t="shared" ref="E39:E46" si="6">IF(ISBLANK(C39),"", (D39-C39+1))</f>
+        <v>2</v>
       </c>
       <c r="F39" s="22" t="s">
         <v>44</v>
@@ -3271,12 +3309,12 @@
     </row>
     <row r="40" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F40" s="22" t="s">
@@ -3285,12 +3323,12 @@
     </row>
     <row r="41" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F41" s="22" t="s">
@@ -3299,12 +3337,12 @@
     </row>
     <row r="42" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F42" s="22" t="s">
@@ -3313,12 +3351,12 @@
     </row>
     <row r="43" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
       <c r="E43" s="21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F43" s="22" t="s">
@@ -3327,20 +3365,46 @@
     </row>
     <row r="44" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
       <c r="E44" s="21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F44" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="47" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated as of 2/22
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan Freeman\Documents\Southern Methodist University - MS in Data Science\Courses\Spring 2018\MSDS 6120 Capstone A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F4C745-5203-3C42-8D8F-723610FA4171}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-76800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>Start Date</t>
   </si>
@@ -174,9 +175,6 @@
   </si>
   <si>
     <t>Meeting with Dr. Engels #1</t>
-  </si>
-  <si>
-    <t>Meeting # 15</t>
   </si>
 </sst>
 </file>
@@ -554,9 +552,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$46</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$45</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -612,66 +610,63 @@
                   <c:v>Meeting # 9</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Meeting with Advisor # 3</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Meeting # 10</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>Meeting with Advisor # 3</c:v>
-                </c:pt>
                 <c:pt idx="20">
+                  <c:v>Meeting with Advisor # 4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Meeting with Dr. Engels #1</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Meeting # 11</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Meeting with Advisor # 4</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Meeting with Dr. Engels #1</c:v>
-                </c:pt>
                 <c:pt idx="23">
+                  <c:v>Meeting with Advisor # 5</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Meeting # 12</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>First Paper Draft Review with Advisor</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>First Paper Draft (A)</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Meeting with Advisor # 6</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>Meeting # 14</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>First Paper Draft Review with Advisor</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>First Paper Draft (A)</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Meeting with Advisor # 6</c:v>
-                </c:pt>
                 <c:pt idx="30">
-                  <c:v>Meeting # 15</c:v>
+                  <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Online Café Talk</c:v>
+                  <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Second Paper Draft (B)</c:v>
+                  <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Third Paper Draft (B)</c:v>
+                  <c:v>Peer Review (B)</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Peer Review (B)</c:v>
+                  <c:v>Final Papers (B)</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Final Papers (B)</c:v>
+                  <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>Poster Presentation (B)</c:v>
+                  <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>Lightning Presentation (B)</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -679,10 +674,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$46</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$45</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
                 </c:pt>
@@ -735,48 +730,45 @@
                   <c:v>43148</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43153</c:v>
+                  <c:v>43156</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43156</c:v>
+                  <c:v>43158</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43158</c:v>
+                  <c:v>43162</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43162</c:v>
+                  <c:v>43165</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43165</c:v>
+                  <c:v>43166</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43166</c:v>
+                  <c:v>43167</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43167</c:v>
+                  <c:v>43169</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43169</c:v>
+                  <c:v>43170</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43170</c:v>
+                  <c:v>43172</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>43172</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43172</c:v>
+                  <c:v>43132</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43132</c:v>
+                  <c:v>43179</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>43179</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>43179</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>43180</c:v>
                 </c:pt>
               </c:numCache>
@@ -1281,9 +1273,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$46</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$45</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -1339,66 +1331,63 @@
                   <c:v>Meeting # 9</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>Meeting with Advisor # 3</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Meeting # 10</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>Meeting with Advisor # 3</c:v>
-                </c:pt>
                 <c:pt idx="20">
+                  <c:v>Meeting with Advisor # 4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Meeting with Dr. Engels #1</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Meeting # 11</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Meeting with Advisor # 4</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Meeting with Dr. Engels #1</c:v>
-                </c:pt>
                 <c:pt idx="23">
+                  <c:v>Meeting with Advisor # 5</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Meeting # 12</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>First Paper Draft Review with Advisor</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>First Paper Draft (A)</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Meeting with Advisor # 6</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>Meeting # 14</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>First Paper Draft Review with Advisor</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>First Paper Draft (A)</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Meeting with Advisor # 6</c:v>
-                </c:pt>
                 <c:pt idx="30">
-                  <c:v>Meeting # 15</c:v>
+                  <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Online Café Talk</c:v>
+                  <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Second Paper Draft (B)</c:v>
+                  <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Third Paper Draft (B)</c:v>
+                  <c:v>Peer Review (B)</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Peer Review (B)</c:v>
+                  <c:v>Final Papers (B)</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Final Papers (B)</c:v>
+                  <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>Poster Presentation (B)</c:v>
+                  <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>Lightning Presentation (B)</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1406,10 +1395,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$46</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$45</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1492,19 +1481,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
@@ -1522,9 +1511,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="38">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2251,15 +2237,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>197946</xdr:rowOff>
+      <xdr:rowOff>7446</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>825500</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>78740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2553,32 +2539,32 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:U55"/>
+  <dimension ref="B1:U54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.75" style="3" customWidth="1"/>
-    <col min="3" max="6" width="15.75" style="3" customWidth="1"/>
-    <col min="7" max="7" width="2.25" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.75" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.25" style="3"/>
+    <col min="1" max="1" width="2.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="3" customWidth="1"/>
+    <col min="3" max="6" width="15.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="3"/>
     <col min="10" max="10" width="1.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="4.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.25" style="3"/>
-    <col min="13" max="13" width="15.25" style="3" customWidth="1"/>
-    <col min="14" max="17" width="11.25" style="3"/>
-    <col min="18" max="19" width="10.75" style="3" customWidth="1"/>
-    <col min="20" max="20" width="11.25" style="3"/>
+    <col min="12" max="12" width="11.1640625" style="3"/>
+    <col min="13" max="13" width="15.1640625" style="3" customWidth="1"/>
+    <col min="14" max="17" width="11.1640625" style="3"/>
+    <col min="18" max="19" width="10.6640625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="11.1640625" style="3"/>
     <col min="21" max="21" width="11.5" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="11.25" style="3"/>
+    <col min="22" max="16384" width="11.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
         <v>38</v>
       </c>
@@ -2589,7 +2575,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
         <v>39</v>
       </c>
@@ -2600,14 +2586,14 @@
       <c r="E2" s="12"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
@@ -2618,7 +2604,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -2631,7 +2617,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2653,7 +2639,7 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -2686,7 +2672,7 @@
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
     </row>
-    <row r="8" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
@@ -2705,7 +2691,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
@@ -2724,7 +2710,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
@@ -2743,7 +2729,7 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="s">
         <v>6</v>
       </c>
@@ -2762,7 +2748,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -2781,7 +2767,7 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
@@ -2800,7 +2786,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="s">
         <v>21</v>
       </c>
@@ -2819,7 +2805,7 @@
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
         <v>16</v>
       </c>
@@ -2838,7 +2824,7 @@
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:21" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
         <v>17</v>
       </c>
@@ -2857,7 +2843,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="s">
         <v>43</v>
       </c>
@@ -2876,7 +2862,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="17" t="s">
         <v>22</v>
       </c>
@@ -2887,7 +2873,7 @@
         <v>43132</v>
       </c>
       <c r="E18" s="21">
-        <f t="shared" ref="E18:E36" si="3">IF(ISBLANK(C18),"", (D18-C18+1))</f>
+        <f t="shared" ref="E18:E35" si="3">IF(ISBLANK(C18),"", (D18-C18+1))</f>
         <v>1</v>
       </c>
       <c r="F18" s="20" t="s">
@@ -2895,7 +2881,7 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17" t="s">
         <v>25</v>
       </c>
@@ -2914,7 +2900,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="17" t="s">
         <v>23</v>
       </c>
@@ -2933,7 +2919,7 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="17" t="s">
         <v>35</v>
       </c>
@@ -2952,7 +2938,7 @@
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="17" t="s">
         <v>26</v>
       </c>
@@ -2971,7 +2957,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="17" t="s">
         <v>24</v>
       </c>
@@ -2990,7 +2976,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="17" t="s">
         <v>28</v>
       </c>
@@ -3009,15 +2995,15 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="18">
-        <v>43153</v>
+        <v>43156</v>
       </c>
       <c r="D25" s="18">
-        <v>43153</v>
+        <v>43156</v>
       </c>
       <c r="E25" s="21">
         <f t="shared" si="3"/>
@@ -3028,15 +3014,15 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C26" s="18">
-        <v>43156</v>
+        <v>43158</v>
       </c>
       <c r="D26" s="18">
-        <v>43156</v>
+        <v>43158</v>
       </c>
       <c r="E26" s="21">
         <f t="shared" si="3"/>
@@ -3047,15 +3033,15 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="17" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C27" s="18">
-        <v>43158</v>
+        <v>43162</v>
       </c>
       <c r="D27" s="18">
-        <v>43158</v>
+        <v>43162</v>
       </c>
       <c r="E27" s="21">
         <f t="shared" si="3"/>
@@ -3066,15 +3052,15 @@
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C28" s="18">
-        <v>43162</v>
+        <v>43165</v>
       </c>
       <c r="D28" s="18">
-        <v>43162</v>
+        <v>43165</v>
       </c>
       <c r="E28" s="21">
         <f t="shared" si="3"/>
@@ -3085,15 +3071,15 @@
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="17" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C29" s="18">
-        <v>43165</v>
+        <v>43166</v>
       </c>
       <c r="D29" s="18">
-        <v>43165</v>
+        <v>43166</v>
       </c>
       <c r="E29" s="21">
         <f t="shared" si="3"/>
@@ -3104,15 +3090,15 @@
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="17" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C30" s="18">
-        <v>43166</v>
+        <v>43167</v>
       </c>
       <c r="D30" s="18">
-        <v>43166</v>
+        <v>43167</v>
       </c>
       <c r="E30" s="21">
         <f t="shared" si="3"/>
@@ -3121,17 +3107,16 @@
       <c r="F30" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="17" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C31" s="18">
-        <v>43167</v>
+        <v>43169</v>
       </c>
       <c r="D31" s="18">
-        <v>43167</v>
+        <v>43169</v>
       </c>
       <c r="E31" s="21">
         <f t="shared" si="3"/>
@@ -3141,15 +3126,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="2:7" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="17" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C32" s="18">
-        <v>43169</v>
+        <v>43170</v>
       </c>
       <c r="D32" s="18">
-        <v>43169</v>
+        <v>43170</v>
       </c>
       <c r="E32" s="21">
         <f t="shared" si="3"/>
@@ -3159,15 +3144,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C33" s="18">
-        <v>43170</v>
+        <v>43172</v>
       </c>
       <c r="D33" s="18">
-        <v>43170</v>
+        <v>43172</v>
       </c>
       <c r="E33" s="21">
         <f t="shared" si="3"/>
@@ -3177,9 +3162,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="17" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C34" s="18">
         <v>43172</v>
@@ -3194,68 +3179,68 @@
       <c r="F34" s="22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="6"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="17" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C35" s="18">
-        <v>43172</v>
+        <v>43132</v>
       </c>
       <c r="D35" s="18">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="E35" s="21">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="F35" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H35" s="6"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
-      <c r="Q35" s="26"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
       <c r="R35" s="7"/>
     </row>
-    <row r="36" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="17" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C36" s="18">
-        <v>43132</v>
+        <v>43179</v>
       </c>
       <c r="D36" s="18">
-        <v>43173</v>
+        <v>43179</v>
       </c>
       <c r="E36" s="21">
-        <f t="shared" si="3"/>
-        <v>42</v>
+        <f t="shared" ref="E36:E37" si="5">IF(ISBLANK(C36),"", (D36-C36+1))</f>
+        <v>1</v>
       </c>
       <c r="F36" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H36" s="7"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="7"/>
-    </row>
-    <row r="37" spans="2:18" s="5" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="17" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C37" s="18">
         <v>43179</v>
@@ -3264,52 +3249,48 @@
         <v>43179</v>
       </c>
       <c r="E37" s="21">
-        <f t="shared" ref="E37:E38" si="5">IF(ISBLANK(C37),"", (D37-C37+1))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F37" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="17" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C38" s="18">
-        <v>43179</v>
+        <v>43180</v>
       </c>
       <c r="D38" s="18">
-        <v>43179</v>
+        <v>43181</v>
       </c>
       <c r="E38" s="21">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" ref="E38:E45" si="6">IF(ISBLANK(C38),"", (D38-C38+1))</f>
+        <v>2</v>
       </c>
       <c r="F38" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="18">
-        <v>43180</v>
-      </c>
-      <c r="D39" s="18">
-        <v>43181</v>
-      </c>
-      <c r="E39" s="21">
-        <f t="shared" ref="E39:E46" si="6">IF(ISBLANK(C39),"", (D39-C39+1))</f>
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="F39" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="17" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
@@ -3321,9 +3302,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -3335,9 +3316,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -3349,9 +3330,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -3363,9 +3344,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
@@ -3377,9 +3358,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -3391,35 +3372,21 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="21" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F46" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:18" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="53" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="54" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="I34:M34"/>
     <mergeCell ref="I35:M35"/>
-    <mergeCell ref="I36:M36"/>
+    <mergeCell ref="N34:Q34"/>
     <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="N36:Q36"/>
     <mergeCell ref="K7:R7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Updated as of 2/25
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a958261cafb92040/DataScience/Capstone/Products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F4C745-5203-3C42-8D8F-723610FA4171}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-76800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15810" windowHeight="6480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
@@ -180,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -676,7 +675,7 @@
             <c:numRef>
               <c:f>'Basic Manual Gantt Chart'!$C$8:$C$45</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
@@ -2535,36 +2534,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:U54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="3" customWidth="1"/>
-    <col min="3" max="6" width="15.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="2.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="3"/>
+    <col min="1" max="1" width="2.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="3" customWidth="1"/>
+    <col min="3" max="6" width="15.625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="2.125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.125" style="3"/>
     <col min="10" max="10" width="1.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="4.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" style="3"/>
-    <col min="13" max="13" width="15.1640625" style="3" customWidth="1"/>
-    <col min="14" max="17" width="11.1640625" style="3"/>
-    <col min="18" max="19" width="10.6640625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" style="3"/>
+    <col min="12" max="12" width="11.125" style="3"/>
+    <col min="13" max="13" width="15.125" style="3" customWidth="1"/>
+    <col min="14" max="17" width="11.125" style="3"/>
+    <col min="18" max="19" width="10.625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="11.125" style="3"/>
     <col min="21" max="21" width="11.5" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="11.1640625" style="3"/>
+    <col min="22" max="16384" width="11.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
         <v>38</v>
       </c>
@@ -2575,7 +2574,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>39</v>
       </c>
@@ -2586,14 +2585,14 @@
       <c r="E2" s="12"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
@@ -2604,7 +2603,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -2617,7 +2616,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2639,7 +2638,7 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -2672,7 +2671,7 @@
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
     </row>
-    <row r="8" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
@@ -2691,7 +2690,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
@@ -2710,7 +2709,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
@@ -2729,7 +2728,7 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
         <v>6</v>
       </c>
@@ -2748,7 +2747,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -2767,7 +2766,7 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
@@ -2786,7 +2785,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>21</v>
       </c>
@@ -2805,7 +2804,7 @@
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
         <v>16</v>
       </c>
@@ -2824,7 +2823,7 @@
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
         <v>17</v>
       </c>
@@ -2843,7 +2842,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>43</v>
       </c>
@@ -2862,7 +2861,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
         <v>22</v>
       </c>
@@ -2881,7 +2880,7 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
         <v>25</v>
       </c>
@@ -2900,7 +2899,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
         <v>23</v>
       </c>
@@ -2919,7 +2918,7 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
         <v>35</v>
       </c>
@@ -2938,7 +2937,7 @@
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>26</v>
       </c>
@@ -2957,7 +2956,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>24</v>
       </c>
@@ -2976,7 +2975,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
         <v>28</v>
       </c>
@@ -2995,7 +2994,7 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
         <v>30</v>
       </c>
@@ -3009,12 +3008,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F25" s="22" t="s">
-        <v>44</v>
+      <c r="F25" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
         <v>27</v>
       </c>
@@ -3033,7 +3032,7 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
         <v>31</v>
       </c>
@@ -3052,7 +3051,7 @@
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
         <v>29</v>
       </c>
@@ -3071,7 +3070,7 @@
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
         <v>49</v>
       </c>
@@ -3090,7 +3089,7 @@
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
         <v>33</v>
       </c>
@@ -3108,7 +3107,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
         <v>47</v>
       </c>
@@ -3126,7 +3125,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="2:7" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
         <v>34</v>
       </c>
@@ -3144,7 +3143,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
         <v>45</v>
       </c>
@@ -3162,7 +3161,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
         <v>36</v>
       </c>
@@ -3191,7 +3190,7 @@
       <c r="Q34" s="26"/>
       <c r="R34" s="7"/>
     </row>
-    <row r="35" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17" t="s">
         <v>7</v>
       </c>
@@ -3220,7 +3219,7 @@
       <c r="Q35" s="25"/>
       <c r="R35" s="7"/>
     </row>
-    <row r="36" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="17" t="s">
         <v>32</v>
       </c>
@@ -3238,7 +3237,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="17" t="s">
         <v>48</v>
       </c>
@@ -3256,7 +3255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
         <v>35</v>
       </c>
@@ -3274,7 +3273,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="17" t="s">
         <v>37</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
         <v>8</v>
       </c>
@@ -3302,7 +3301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
         <v>9</v>
       </c>
@@ -3316,7 +3315,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="17" t="s">
         <v>10</v>
       </c>
@@ -3330,7 +3329,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="17" t="s">
         <v>11</v>
       </c>
@@ -3344,7 +3343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="17" t="s">
         <v>12</v>
       </c>
@@ -3358,7 +3357,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="17" t="s">
         <v>13</v>
       </c>
@@ -3372,15 +3371,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="I34:M34"/>

</xml_diff>

<commit_message>
Updated as of 3/3/18
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15810" windowHeight="6480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19485" windowHeight="6480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>Start Date</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Meeting # 10</t>
   </si>
   <si>
-    <t>Meeting with Advisor # 6</t>
-  </si>
-  <si>
     <t>Meeting # 11</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
   </si>
   <si>
     <t>Meeting with Advisor # 5</t>
-  </si>
-  <si>
-    <t>Meeting # 14</t>
   </si>
   <si>
     <t>Meeting with Dr. Engels #1</t>
@@ -551,9 +545,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$45</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$43</c:f>
               <c:strCache>
-                <c:ptCount val="38"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -612,60 +606,54 @@
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>Meeting with Dr. Engels #1</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>Meeting # 10</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Meeting with Advisor # 4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Meeting with Dr. Engels #1</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>Meeting # 11</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>Meeting # 12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>First Paper Draft Review with Advisor</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>First Paper Draft (A)</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>Meeting # 12</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>First Paper Draft Review with Advisor</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>First Paper Draft (A)</c:v>
-                </c:pt>
                 <c:pt idx="28">
-                  <c:v>Meeting with Advisor # 6</c:v>
+                  <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Meeting # 14</c:v>
+                  <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Online Café Talk</c:v>
+                  <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Second Paper Draft (B)</c:v>
+                  <c:v>Peer Review (B)</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Third Paper Draft (B)</c:v>
+                  <c:v>Final Papers (B)</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Peer Review (B)</c:v>
+                  <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Final Papers (B)</c:v>
+                  <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Poster Presentation (B)</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Lightning Presentation (B)</c:v>
-                </c:pt>
-                <c:pt idx="37">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -673,10 +661,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$45</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
                 </c:pt>
@@ -732,42 +720,36 @@
                   <c:v>43156</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43158</c:v>
+                  <c:v>43162</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43162</c:v>
+                  <c:v>43166</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43165</c:v>
+                  <c:v>43167</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43166</c:v>
+                  <c:v>43169</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43167</c:v>
+                  <c:v>43170</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43169</c:v>
+                  <c:v>43172</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43170</c:v>
+                  <c:v>43172</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43172</c:v>
+                  <c:v>43132</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43172</c:v>
+                  <c:v>43179</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43132</c:v>
+                  <c:v>43179</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43179</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>43179</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>43180</c:v>
                 </c:pt>
               </c:numCache>
@@ -1272,9 +1254,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$45</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$43</c:f>
               <c:strCache>
-                <c:ptCount val="38"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -1333,60 +1315,54 @@
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>Meeting with Dr. Engels #1</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>Meeting # 10</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Meeting with Advisor # 4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Meeting with Dr. Engels #1</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>Meeting # 11</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>Meeting # 12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>First Paper Draft Review with Advisor</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>First Paper Draft (A)</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>Meeting # 12</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>First Paper Draft Review with Advisor</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>First Paper Draft (A)</c:v>
-                </c:pt>
                 <c:pt idx="28">
-                  <c:v>Meeting with Advisor # 6</c:v>
+                  <c:v>Online Café Talk</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Meeting # 14</c:v>
+                  <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Online Café Talk</c:v>
+                  <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Second Paper Draft (B)</c:v>
+                  <c:v>Peer Review (B)</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Third Paper Draft (B)</c:v>
+                  <c:v>Final Papers (B)</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Peer Review (B)</c:v>
+                  <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Final Papers (B)</c:v>
+                  <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Poster Presentation (B)</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Lightning Presentation (B)</c:v>
-                </c:pt>
-                <c:pt idx="37">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1394,10 +1370,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$45</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1474,22 +1450,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
@@ -1504,12 +1480,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2243,7 +2213,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>78740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2538,7 +2508,7 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:U54"/>
+  <dimension ref="B1:U52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
@@ -2565,10 +2535,10 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -2576,10 +2546,10 @@
     </row>
     <row r="2" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -2611,7 +2581,7 @@
         <v>43332</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
@@ -2686,7 +2656,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -2705,7 +2675,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -2724,7 +2694,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -2743,7 +2713,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -2762,7 +2732,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -2781,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -2800,7 +2770,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -2819,7 +2789,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" s="4"/>
     </row>
@@ -2838,13 +2808,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="C17" s="18">
         <v>43131</v>
@@ -2857,11 +2827,11 @@
         <v>1</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
         <v>22</v>
       </c>
@@ -2872,15 +2842,15 @@
         <v>43132</v>
       </c>
       <c r="E18" s="21">
-        <f t="shared" ref="E18:E35" si="3">IF(ISBLANK(C18),"", (D18-C18+1))</f>
+        <f t="shared" ref="E18:E33" si="3">IF(ISBLANK(C18),"", (D18-C18+1))</f>
         <v>1</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
         <v>25</v>
       </c>
@@ -2895,11 +2865,11 @@
         <v>1</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
         <v>23</v>
       </c>
@@ -2914,13 +2884,13 @@
         <v>1</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="18">
         <v>43138</v>
@@ -2933,11 +2903,11 @@
         <v>2</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>26</v>
       </c>
@@ -2952,11 +2922,11 @@
         <v>1</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>24</v>
       </c>
@@ -2971,11 +2941,11 @@
         <v>1</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
         <v>28</v>
       </c>
@@ -2990,11 +2960,11 @@
         <v>1</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
         <v>30</v>
       </c>
@@ -3009,273 +2979,263 @@
         <v>1</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="18">
-        <v>43158</v>
+        <v>43162</v>
       </c>
       <c r="D26" s="18">
-        <v>43158</v>
+        <v>43162</v>
       </c>
       <c r="E26" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F26" s="22" t="s">
-        <v>44</v>
+      <c r="F26" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C27" s="18">
-        <v>43162</v>
+        <v>43166</v>
       </c>
       <c r="D27" s="18">
-        <v>43162</v>
+        <v>43166</v>
       </c>
       <c r="E27" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C28" s="18">
-        <v>43165</v>
+        <v>43167</v>
       </c>
       <c r="D28" s="18">
-        <v>43165</v>
+        <v>43167</v>
       </c>
       <c r="E28" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C29" s="18">
-        <v>43166</v>
+        <v>43169</v>
       </c>
       <c r="D29" s="18">
-        <v>43166</v>
+        <v>43169</v>
       </c>
       <c r="E29" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="18">
-        <v>43167</v>
+        <v>43170</v>
       </c>
       <c r="D30" s="18">
-        <v>43167</v>
+        <v>43170</v>
       </c>
       <c r="E30" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C31" s="18">
-        <v>43169</v>
+        <v>43172</v>
       </c>
       <c r="D31" s="18">
-        <v>43169</v>
+        <v>43172</v>
       </c>
       <c r="E31" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C32" s="18">
-        <v>43170</v>
+        <v>43172</v>
       </c>
       <c r="D32" s="18">
-        <v>43170</v>
+        <v>43172</v>
       </c>
       <c r="E32" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="7"/>
     </row>
     <row r="33" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C33" s="18">
-        <v>43172</v>
+        <v>43132</v>
       </c>
       <c r="D33" s="18">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="E33" s="21">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="7"/>
     </row>
     <row r="34" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C34" s="18">
-        <v>43172</v>
+        <v>43179</v>
       </c>
       <c r="D34" s="18">
-        <v>43172</v>
+        <v>43179</v>
       </c>
       <c r="E34" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E34:E35" si="5">IF(ISBLANK(C34),"", (D34-C34+1))</f>
         <v>1</v>
       </c>
       <c r="F34" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="7"/>
-    </row>
-    <row r="35" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="17" t="s">
-        <v>7</v>
-      </c>
       <c r="C35" s="18">
-        <v>43132</v>
+        <v>43179</v>
       </c>
       <c r="D35" s="18">
-        <v>43173</v>
+        <v>43179</v>
       </c>
       <c r="E35" s="21">
-        <f t="shared" si="3"/>
-        <v>42</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="H35" s="7"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="7"/>
-    </row>
-    <row r="36" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C36" s="18">
-        <v>43179</v>
+        <v>43180</v>
       </c>
       <c r="D36" s="18">
-        <v>43179</v>
+        <v>43181</v>
       </c>
       <c r="E36" s="21">
-        <f t="shared" ref="E36:E37" si="5">IF(ISBLANK(C36),"", (D36-C36+1))</f>
-        <v>1</v>
+        <f t="shared" ref="E36:E43" si="6">IF(ISBLANK(C36),"", (D36-C36+1))</f>
+        <v>2</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="18">
-        <v>43179</v>
-      </c>
-      <c r="D37" s="18">
-        <v>43179</v>
-      </c>
-      <c r="E37" s="21">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="F37" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="18">
-        <v>43180</v>
-      </c>
-      <c r="D38" s="18">
-        <v>43181</v>
-      </c>
-      <c r="E38" s="21">
-        <f t="shared" ref="E38:E45" si="6">IF(ISBLANK(C38),"", (D38-C38+1))</f>
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="F38" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="17" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -3284,12 +3244,12 @@
         <v/>
       </c>
       <c r="F39" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
@@ -3298,12 +3258,12 @@
         <v/>
       </c>
       <c r="F40" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -3312,12 +3272,12 @@
         <v/>
       </c>
       <c r="F41" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -3326,12 +3286,12 @@
         <v/>
       </c>
       <c r="F42" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -3340,37 +3300,11 @@
         <v/>
       </c>
       <c r="F43" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="21" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="21" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F45" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3378,14 +3312,12 @@
     <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="I34:M34"/>
-    <mergeCell ref="I35:M35"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="I32:M32"/>
+    <mergeCell ref="I33:M33"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="N33:Q33"/>
     <mergeCell ref="K7:R7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Updated as of 3/6
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>Start Date</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Meeting with Dr. Engels #1</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor #4(Sudip &amp; Craig in person)</t>
+  </si>
+  <si>
+    <t>Meeting #10</t>
   </si>
 </sst>
 </file>
@@ -545,9 +551,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$43</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$45</c:f>
               <c:strCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -606,54 +612,60 @@
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>Meeting with Advisor #4(Sudip &amp; Craig in person)</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Meeting #10</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>Meeting with Dr. Engels #1</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>Meeting # 10</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>Meeting with Advisor # 4</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>Meeting # 11</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>Meeting # 12</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>First Paper Draft Review with Advisor</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -723,13 +735,13 @@
                   <c:v>43162</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>43165</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43165</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>43166</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43167</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43169</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>43170</c:v>
@@ -1254,9 +1266,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$43</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$45</c:f>
               <c:strCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -1315,54 +1327,60 @@
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>Meeting with Advisor #4(Sudip &amp; Craig in person)</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Meeting #10</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>Meeting with Dr. Engels #1</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>Meeting # 10</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>Meeting with Advisor # 4</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>Meeting # 11</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>Meeting # 12</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>First Paper Draft Review with Advisor</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>Online Café Talk</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -2510,14 +2528,14 @@
   </sheetPr>
   <dimension ref="B1:U52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.75" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="15.625" style="3" customWidth="1"/>
     <col min="7" max="7" width="2.125" style="3" customWidth="1"/>
     <col min="8" max="8" width="27.625" style="3" customWidth="1"/>
@@ -3004,50 +3022,50 @@
     </row>
     <row r="27" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C27" s="18">
-        <v>43166</v>
+        <v>43165</v>
       </c>
       <c r="D27" s="18">
-        <v>43166</v>
+        <v>43165</v>
       </c>
       <c r="E27" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F27" s="22" t="s">
-        <v>43</v>
+      <c r="F27" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C28" s="18">
-        <v>43167</v>
+        <v>43165</v>
       </c>
       <c r="D28" s="18">
-        <v>43167</v>
+        <v>43165</v>
       </c>
       <c r="E28" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F28" s="22" t="s">
-        <v>43</v>
+      <c r="F28" s="20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C29" s="18">
-        <v>43169</v>
+        <v>43166</v>
       </c>
       <c r="D29" s="18">
-        <v>43169</v>
+        <v>43166</v>
       </c>
       <c r="E29" s="21">
         <f t="shared" si="3"/>
@@ -3059,7 +3077,7 @@
     </row>
     <row r="30" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="18">
         <v>43170</v>
@@ -3077,7 +3095,7 @@
     </row>
     <row r="31" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C31" s="18">
         <v>43172</v>
@@ -3095,7 +3113,7 @@
     </row>
     <row r="32" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C32" s="18">
         <v>43172</v>
@@ -3124,7 +3142,7 @@
     </row>
     <row r="33" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C33" s="18">
         <v>43132</v>
@@ -3153,7 +3171,7 @@
     </row>
     <row r="34" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C34" s="18">
         <v>43179</v>
@@ -3171,7 +3189,7 @@
     </row>
     <row r="35" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="17" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C35" s="18">
         <v>43179</v>
@@ -3189,7 +3207,7 @@
     </row>
     <row r="36" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C36" s="18">
         <v>43180</v>
@@ -3207,7 +3225,7 @@
     </row>
     <row r="37" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="17" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -3221,7 +3239,7 @@
     </row>
     <row r="38" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -3235,7 +3253,7 @@
     </row>
     <row r="39" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="17" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -3249,7 +3267,7 @@
     </row>
     <row r="40" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
@@ -3263,7 +3281,7 @@
     </row>
     <row r="41" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -3277,7 +3295,7 @@
     </row>
     <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -3291,7 +3309,7 @@
     </row>
     <row r="43" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -3303,8 +3321,16 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="46" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated as of 3/15/18
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a958261cafb92040/DataScience/Capstone/Products/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95B2C7C-341C-CF49-AF53-8239AF158718}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19485" windowHeight="6480" tabRatio="500"/>
+    <workbookView xWindow="-76800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>Start Date</t>
   </si>
@@ -113,15 +114,9 @@
     <t>Meeting # 8</t>
   </si>
   <si>
-    <t>Meeting with Advisor # 4</t>
-  </si>
-  <si>
     <t>Meeting # 9</t>
   </si>
   <si>
-    <t>Meeting # 10</t>
-  </si>
-  <si>
     <t>Meeting # 11</t>
   </si>
   <si>
@@ -131,9 +126,6 @@
     <t>Online Café Talk</t>
   </si>
   <si>
-    <t>First Paper Draft Review with Advisor</t>
-  </si>
-  <si>
     <t>Second Paper Draft (B)</t>
   </si>
   <si>
@@ -158,28 +150,40 @@
     <t>Not Started</t>
   </si>
   <si>
-    <t>Meeting # 13</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blockchain for Anti-Money Laundering                     </t>
   </si>
   <si>
     <t>Meeting with Advisor # 5</t>
   </si>
   <si>
-    <t>Meeting with Dr. Engels #1</t>
-  </si>
-  <si>
     <t>Meeting with Advisor #4(Sudip &amp; Craig in person)</t>
   </si>
   <si>
     <t>Meeting #10</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor # 6</t>
+  </si>
+  <si>
+    <t>Meeting 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting to Introduce John </t>
+  </si>
+  <si>
+    <t>Online Café Talk (Dan &amp; Tim)</t>
+  </si>
+  <si>
+    <t>Online Café Talk (Sudip)</t>
+  </si>
+  <si>
+    <t>Meeting with Dr. Engels &amp; Advisors  #1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -395,7 +399,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -451,6 +455,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -618,34 +625,34 @@
                   <c:v>Meeting #10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Meeting with Dr. Engels #1</c:v>
+                  <c:v>Meeting with Dr. Engels &amp; Advisors  #1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Meeting # 10</c:v>
+                  <c:v>Meeting # 11</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Meeting with Advisor # 4</c:v>
+                  <c:v>Meeting # 12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Meeting # 11</c:v>
+                  <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Meeting # 12</c:v>
+                  <c:v>Online Café Talk (Dan &amp; Tim)</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>First Paper Draft Review with Advisor</c:v>
+                  <c:v>Online Café Talk (Sudip)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>First Paper Draft (A)</c:v>
+                  <c:v>Meeting to Introduce John </c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Meeting # 13</c:v>
+                  <c:v>Meeting 13</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Online Café Talk</c:v>
+                  <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>Second Paper Draft (B)</c:v>
@@ -675,7 +682,7 @@
             <c:numRef>
               <c:f>'Basic Manual Gantt Chart'!$C$8:$C$43</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
@@ -747,22 +754,28 @@
                   <c:v>43170</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43172</c:v>
+                  <c:v>43173</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43172</c:v>
+                  <c:v>43132</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43132</c:v>
+                  <c:v>43179</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43179</c:v>
+                  <c:v>43180</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43179</c:v>
+                  <c:v>43181</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43180</c:v>
+                  <c:v>43186</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43190</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1333,34 +1346,34 @@
                   <c:v>Meeting #10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Meeting with Dr. Engels #1</c:v>
+                  <c:v>Meeting with Dr. Engels &amp; Advisors  #1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Meeting # 10</c:v>
+                  <c:v>Meeting # 11</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Meeting with Advisor # 4</c:v>
+                  <c:v>Meeting # 12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Meeting # 11</c:v>
+                  <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Meeting # 12</c:v>
+                  <c:v>Online Café Talk (Dan &amp; Tim)</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>First Paper Draft Review with Advisor</c:v>
+                  <c:v>Online Café Talk (Sudip)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>First Paper Draft (A)</c:v>
+                  <c:v>Meeting to Introduce John </c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>Meeting with Advisor # 5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Meeting # 13</c:v>
+                  <c:v>Meeting 13</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Online Café Talk</c:v>
+                  <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>Second Paper Draft (B)</c:v>
@@ -1465,10 +1478,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>1</c:v>
@@ -1477,13 +1490,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
@@ -2522,65 +2535,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:U52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="34.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="15.625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="2.125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.125" style="3"/>
+    <col min="1" max="1" width="2.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="3"/>
     <col min="10" max="10" width="1.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="4.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.125" style="3"/>
-    <col min="13" max="13" width="15.125" style="3" customWidth="1"/>
-    <col min="14" max="17" width="11.125" style="3"/>
-    <col min="18" max="19" width="10.625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="11.125" style="3"/>
+    <col min="12" max="12" width="11.1640625" style="3"/>
+    <col min="13" max="13" width="15.1640625" style="3" customWidth="1"/>
+    <col min="14" max="17" width="11.1640625" style="3"/>
+    <col min="18" max="19" width="10.6640625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="11.1640625" style="3"/>
     <col min="21" max="21" width="11.5" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="11.125" style="3"/>
+    <col min="22" max="16384" width="11.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
@@ -2591,7 +2604,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -2599,12 +2612,12 @@
         <v>43332</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2626,7 +2639,7 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -2650,16 +2663,16 @@
         <f>C8</f>
         <v>43118</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-    </row>
-    <row r="8" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+    </row>
+    <row r="8" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
@@ -2674,11 +2687,11 @@
         <v>1</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
@@ -2693,11 +2706,11 @@
         <v>1</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
@@ -2712,11 +2725,11 @@
         <v>1</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="s">
         <v>6</v>
       </c>
@@ -2731,11 +2744,11 @@
         <v>14</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -2750,11 +2763,11 @@
         <v>1</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
@@ -2769,11 +2782,11 @@
         <v>1</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="s">
         <v>21</v>
       </c>
@@ -2788,11 +2801,11 @@
         <v>8</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
         <v>16</v>
       </c>
@@ -2807,11 +2820,11 @@
         <v>1</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
         <v>17</v>
       </c>
@@ -2826,13 +2839,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C17" s="18">
         <v>43131</v>
@@ -2845,11 +2858,11 @@
         <v>1</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="17" t="s">
         <v>22</v>
       </c>
@@ -2860,15 +2873,15 @@
         <v>43132</v>
       </c>
       <c r="E18" s="21">
-        <f t="shared" ref="E18:E33" si="3">IF(ISBLANK(C18),"", (D18-C18+1))</f>
+        <f t="shared" ref="E18:E35" si="3">IF(ISBLANK(C18),"", (D18-C18+1))</f>
         <v>1</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17" t="s">
         <v>25</v>
       </c>
@@ -2883,11 +2896,11 @@
         <v>1</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="17" t="s">
         <v>23</v>
       </c>
@@ -2902,13 +2915,13 @@
         <v>1</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="18">
         <v>43138</v>
@@ -2921,11 +2934,11 @@
         <v>2</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="17" t="s">
         <v>26</v>
       </c>
@@ -2940,11 +2953,11 @@
         <v>1</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="17" t="s">
         <v>24</v>
       </c>
@@ -2959,11 +2972,11 @@
         <v>1</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="17" t="s">
         <v>28</v>
       </c>
@@ -2978,13 +2991,13 @@
         <v>1</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="18">
         <v>43156</v>
@@ -2997,11 +3010,11 @@
         <v>1</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="17" t="s">
         <v>27</v>
       </c>
@@ -3016,13 +3029,13 @@
         <v>1</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C27" s="18">
         <v>43165</v>
@@ -3035,13 +3048,13 @@
         <v>1</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C28" s="18">
         <v>43165</v>
@@ -3054,12 +3067,12 @@
         <v>1</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C29" s="18">
         <v>43166</v>
@@ -3071,13 +3084,13 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F29" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="18">
         <v>43170</v>
@@ -3089,171 +3102,212 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F30" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C31" s="18">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="D31" s="18">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="E31" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F31" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="7"/>
+    </row>
+    <row r="32" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="17" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C32" s="18">
-        <v>43172</v>
+        <v>43132</v>
       </c>
       <c r="D32" s="18">
-        <v>43172</v>
+        <v>43173</v>
       </c>
       <c r="E32" s="21">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="F32" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
+        <v>42</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
       <c r="N32" s="26"/>
       <c r="O32" s="26"/>
       <c r="P32" s="26"/>
       <c r="Q32" s="26"/>
       <c r="R32" s="7"/>
     </row>
-    <row r="33" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="17" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C33" s="18">
-        <v>43132</v>
+        <v>43179</v>
       </c>
       <c r="D33" s="18">
-        <v>43173</v>
+        <v>43179</v>
       </c>
       <c r="E33" s="21">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="7"/>
+    </row>
+    <row r="34" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="18">
+        <v>43180</v>
+      </c>
+      <c r="D34" s="18">
+        <v>43180</v>
+      </c>
+      <c r="E34" s="21">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" s="7"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="18">
+        <v>43181</v>
+      </c>
+      <c r="D35" s="18">
+        <v>43181</v>
+      </c>
+      <c r="E35" s="21">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="7"/>
+    </row>
+    <row r="36" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="7"/>
-    </row>
-    <row r="34" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="18">
-        <v>43179</v>
-      </c>
-      <c r="D34" s="18">
-        <v>43179</v>
-      </c>
-      <c r="E34" s="21">
-        <f t="shared" ref="E34:E35" si="5">IF(ISBLANK(C34),"", (D34-C34+1))</f>
+      <c r="C36" s="18">
+        <v>43186</v>
+      </c>
+      <c r="D36" s="18">
+        <v>43186</v>
+      </c>
+      <c r="E36" s="21">
+        <f t="shared" ref="E36" si="5">IF(ISBLANK(C36),"", (D36-C36+1))</f>
         <v>1</v>
       </c>
-      <c r="F34" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="18">
-        <v>43179</v>
-      </c>
-      <c r="D35" s="18">
-        <v>43179</v>
-      </c>
-      <c r="E35" s="21">
-        <f t="shared" si="5"/>
+      <c r="F36" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="18">
+        <v>43190</v>
+      </c>
+      <c r="D37" s="18">
+        <v>43190</v>
+      </c>
+      <c r="E37" s="21">
+        <f t="shared" ref="E37:E43" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
         <v>1</v>
       </c>
-      <c r="F35" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="18">
-        <v>43180</v>
-      </c>
-      <c r="D36" s="18">
-        <v>43181</v>
-      </c>
-      <c r="E36" s="21">
-        <f t="shared" ref="E36:E43" si="6">IF(ISBLANK(C36),"", (D36-C36+1))</f>
-        <v>2</v>
-      </c>
-      <c r="F36" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="21" t="str">
+      <c r="F37" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="18">
+        <v>43193</v>
+      </c>
+      <c r="D38" s="18">
+        <v>43193</v>
+      </c>
+      <c r="E38" s="21">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="21" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -3262,10 +3316,10 @@
         <v/>
       </c>
       <c r="F39" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="17" t="s">
         <v>8</v>
       </c>
@@ -3276,10 +3330,10 @@
         <v/>
       </c>
       <c r="F40" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="17" t="s">
         <v>9</v>
       </c>
@@ -3290,10 +3344,10 @@
         <v/>
       </c>
       <c r="F41" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="17" t="s">
         <v>10</v>
       </c>
@@ -3304,10 +3358,10 @@
         <v/>
       </c>
       <c r="F42" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="17" t="s">
         <v>11</v>
       </c>
@@ -3318,32 +3372,32 @@
         <v/>
       </c>
       <c r="F43" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="I31:M31"/>
     <mergeCell ref="I32:M32"/>
-    <mergeCell ref="I33:M33"/>
+    <mergeCell ref="N31:Q31"/>
     <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="N33:Q33"/>
     <mergeCell ref="K7:R7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Updated as of 3/22
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a958261cafb92040/DataScience/Capstone/Products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95B2C7C-341C-CF49-AF53-8239AF158718}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-76800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19485" windowHeight="6480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
@@ -153,9 +152,6 @@
     <t xml:space="preserve">Blockchain for Anti-Money Laundering                     </t>
   </si>
   <si>
-    <t>Meeting with Advisor # 5</t>
-  </si>
-  <si>
     <t>Meeting with Advisor #4(Sudip &amp; Craig in person)</t>
   </si>
   <si>
@@ -165,25 +161,28 @@
     <t>Meeting with Advisor # 6</t>
   </si>
   <si>
-    <t>Meeting 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meeting to Introduce John </t>
-  </si>
-  <si>
-    <t>Online Café Talk (Dan &amp; Tim)</t>
-  </si>
-  <si>
-    <t>Online Café Talk (Sudip)</t>
-  </si>
-  <si>
     <t>Meeting with Dr. Engels &amp; Advisors  #1</t>
+  </si>
+  <si>
+    <t>Online Café Talk (Dan)</t>
+  </si>
+  <si>
+    <t>Online Café Talk (Sudip &amp; Tim)</t>
+  </si>
+  <si>
+    <t>Meeting # 13</t>
+  </si>
+  <si>
+    <t>Meeting #14</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor (Pablo) # 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -637,19 +636,19 @@
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Online Café Talk (Dan &amp; Tim)</c:v>
+                  <c:v>Online Café Talk (Dan)</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Online Café Talk (Sudip)</c:v>
+                  <c:v>Online Café Talk (Sudip &amp; Tim)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Meeting to Introduce John </c:v>
+                  <c:v>Meeting # 13</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Meeting with Advisor # 5</c:v>
+                  <c:v>Meeting with Advisor (Pablo) # 5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Meeting 13</c:v>
+                  <c:v>Meeting #14</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>Meeting with Advisor # 6</c:v>
@@ -682,7 +681,7 @@
             <c:numRef>
               <c:f>'Basic Manual Gantt Chart'!$C$8:$C$43</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
@@ -769,7 +768,7 @@
                   <c:v>43181</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43186</c:v>
+                  <c:v>43183</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>43190</c:v>
@@ -1358,19 +1357,19 @@
                   <c:v>First Paper Draft (A)</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Online Café Talk (Dan &amp; Tim)</c:v>
+                  <c:v>Online Café Talk (Dan)</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Online Café Talk (Sudip)</c:v>
+                  <c:v>Online Café Talk (Sudip &amp; Tim)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Meeting to Introduce John </c:v>
+                  <c:v>Meeting # 13</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Meeting with Advisor # 5</c:v>
+                  <c:v>Meeting with Advisor (Pablo) # 5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Meeting 13</c:v>
+                  <c:v>Meeting #14</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>Meeting with Advisor # 6</c:v>
@@ -2535,36 +2534,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:U52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="15.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="2.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="3"/>
+    <col min="1" max="1" width="2.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="2.125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.125" style="3"/>
     <col min="10" max="10" width="1.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="4.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" style="3"/>
-    <col min="13" max="13" width="15.1640625" style="3" customWidth="1"/>
-    <col min="14" max="17" width="11.1640625" style="3"/>
-    <col min="18" max="19" width="10.6640625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" style="3"/>
+    <col min="12" max="12" width="11.125" style="3"/>
+    <col min="13" max="13" width="15.125" style="3" customWidth="1"/>
+    <col min="14" max="17" width="11.125" style="3"/>
+    <col min="18" max="19" width="10.625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="11.125" style="3"/>
     <col min="21" max="21" width="11.5" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="11.1640625" style="3"/>
+    <col min="22" max="16384" width="11.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
         <v>34</v>
       </c>
@@ -2575,7 +2574,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>35</v>
       </c>
@@ -2586,14 +2585,14 @@
       <c r="E2" s="12"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
@@ -2604,7 +2603,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="2:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -2617,7 +2616,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2639,7 +2638,7 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -2672,7 +2671,7 @@
       <c r="Q7" s="28"/>
       <c r="R7" s="28"/>
     </row>
-    <row r="8" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
@@ -2691,7 +2690,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
@@ -2710,7 +2709,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
@@ -2729,7 +2728,7 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
         <v>6</v>
       </c>
@@ -2748,7 +2747,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -2767,7 +2766,7 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
@@ -2786,7 +2785,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>21</v>
       </c>
@@ -2805,7 +2804,7 @@
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
         <v>16</v>
       </c>
@@ -2824,7 +2823,7 @@
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
         <v>17</v>
       </c>
@@ -2843,7 +2842,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>39</v>
       </c>
@@ -2862,7 +2861,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
         <v>22</v>
       </c>
@@ -2881,7 +2880,7 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
         <v>25</v>
       </c>
@@ -2900,7 +2899,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
         <v>23</v>
       </c>
@@ -2919,7 +2918,7 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
         <v>32</v>
       </c>
@@ -2938,7 +2937,7 @@
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>26</v>
       </c>
@@ -2957,7 +2956,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>24</v>
       </c>
@@ -2976,7 +2975,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
         <v>28</v>
       </c>
@@ -2995,7 +2994,7 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
         <v>29</v>
       </c>
@@ -3014,7 +3013,7 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
         <v>27</v>
       </c>
@@ -3033,9 +3032,9 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="18">
         <v>43165</v>
@@ -3052,9 +3051,9 @@
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="18">
         <v>43165</v>
@@ -3070,9 +3069,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C29" s="18">
         <v>43166</v>
@@ -3088,7 +3087,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
         <v>30</v>
       </c>
@@ -3106,7 +3105,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
         <v>31</v>
       </c>
@@ -3135,7 +3134,7 @@
       <c r="Q31" s="27"/>
       <c r="R31" s="7"/>
     </row>
-    <row r="32" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
         <v>7</v>
       </c>
@@ -3164,9 +3163,9 @@
       <c r="Q32" s="26"/>
       <c r="R32" s="7"/>
     </row>
-    <row r="33" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C33" s="18">
         <v>43179</v>
@@ -3178,8 +3177,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F33" s="22" t="s">
-        <v>40</v>
+      <c r="F33" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="24"/>
@@ -3193,9 +3192,9 @@
       <c r="Q33" s="24"/>
       <c r="R33" s="7"/>
     </row>
-    <row r="34" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C34" s="18">
         <v>43180</v>
@@ -3207,8 +3206,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F34" s="22" t="s">
-        <v>40</v>
+      <c r="F34" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="24"/>
@@ -3222,9 +3221,9 @@
       <c r="Q34" s="24"/>
       <c r="R34" s="7"/>
     </row>
-    <row r="35" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35" s="18">
         <v>43181</v>
@@ -3236,8 +3235,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F35" s="22" t="s">
-        <v>40</v>
+      <c r="F35" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="24"/>
@@ -3251,15 +3250,15 @@
       <c r="Q35" s="24"/>
       <c r="R35" s="7"/>
     </row>
-    <row r="36" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="17" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C36" s="18">
-        <v>43186</v>
+        <v>43183</v>
       </c>
       <c r="D36" s="18">
-        <v>43186</v>
+        <v>43183</v>
       </c>
       <c r="E36" s="21">
         <f t="shared" ref="E36" si="5">IF(ISBLANK(C36),"", (D36-C36+1))</f>
@@ -3269,9 +3268,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C37" s="18">
         <v>43190</v>
@@ -3287,9 +3286,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" s="18">
         <v>43193</v>
@@ -3305,7 +3304,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="17" t="s">
         <v>33</v>
       </c>
@@ -3319,7 +3318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
         <v>8</v>
       </c>
@@ -3333,7 +3332,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
         <v>9</v>
       </c>
@@ -3347,7 +3346,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="17" t="s">
         <v>10</v>
       </c>
@@ -3361,7 +3360,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="17" t="s">
         <v>11</v>
       </c>
@@ -3375,23 +3374,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="I31:M31"/>

</xml_diff>

<commit_message>
Updated as of 3/25/18
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19485" windowHeight="6480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -2541,7 +2541,7 @@
   <dimension ref="B1:U52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3264,8 +3264,8 @@
         <f t="shared" ref="E36" si="5">IF(ISBLANK(C36),"", (D36-C36+1))</f>
         <v>1</v>
       </c>
-      <c r="F36" s="22" t="s">
-        <v>40</v>
+      <c r="F36" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated as of 4/10
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15810" windowHeight="6480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>Start Date</t>
   </si>
@@ -152,18 +152,12 @@
     <t xml:space="preserve">Blockchain for Anti-Money Laundering                     </t>
   </si>
   <si>
-    <t>Meeting with Advisor #4(Sudip &amp; Craig in person)</t>
-  </si>
-  <si>
     <t>Meeting #10</t>
   </si>
   <si>
     <t>Meeting with Advisor # 6</t>
   </si>
   <si>
-    <t>Meeting with Dr. Engels &amp; Advisors  #1</t>
-  </si>
-  <si>
     <t>Online Café Talk (Dan)</t>
   </si>
   <si>
@@ -176,7 +170,16 @@
     <t>Meeting #14</t>
   </si>
   <si>
-    <t>Meeting with Advisor (Pablo) # 5</t>
+    <t>Meeting with Dr. Engels &amp; Advisors  #5</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor (Pablo) # 1</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor (Pablo) # 2</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor #4 (Sudip &amp; Craig in person)</t>
   </si>
 </sst>
 </file>
@@ -557,9 +560,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$45</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$46</c:f>
               <c:strCache>
-                <c:ptCount val="38"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -618,13 +621,13 @@
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Meeting with Advisor #4(Sudip &amp; Craig in person)</c:v>
+                  <c:v>Meeting with Advisor #4 (Sudip &amp; Craig in person)</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Meeting #10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Meeting with Dr. Engels &amp; Advisors  #1</c:v>
+                  <c:v>Meeting with Dr. Engels &amp; Advisors  #5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>Meeting # 11</c:v>
@@ -645,33 +648,36 @@
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Meeting with Advisor (Pablo) # 5</c:v>
+                  <c:v>Meeting with Advisor (Pablo) # 1</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>Meeting #14</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>Meeting with Advisor (Pablo) # 2</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -679,10 +685,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$43</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
                 </c:pt>
@@ -774,7 +780,10 @@
                   <c:v>43190</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>43193</c:v>
+                  <c:v>43200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1278,9 +1287,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$45</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$46</c:f>
               <c:strCache>
-                <c:ptCount val="38"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -1339,13 +1348,13 @@
                   <c:v>Meeting with Advisor # 3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Meeting with Advisor #4(Sudip &amp; Craig in person)</c:v>
+                  <c:v>Meeting with Advisor #4 (Sudip &amp; Craig in person)</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Meeting #10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Meeting with Dr. Engels &amp; Advisors  #1</c:v>
+                  <c:v>Meeting with Dr. Engels &amp; Advisors  #5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>Meeting # 11</c:v>
@@ -1366,33 +1375,36 @@
                   <c:v>Meeting # 13</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Meeting with Advisor (Pablo) # 5</c:v>
+                  <c:v>Meeting with Advisor (Pablo) # 1</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>Meeting #14</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>Meeting with Advisor (Pablo) # 2</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1400,10 +1412,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$43</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$44</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1498,7 +1510,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
@@ -1510,6 +1522,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2243,7 +2258,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>78740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2538,10 +2553,10 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:U52"/>
+  <dimension ref="B1:U53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3034,7 +3049,7 @@
     </row>
     <row r="27" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C27" s="18">
         <v>43165</v>
@@ -3053,7 +3068,7 @@
     </row>
     <row r="28" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="18">
         <v>43165</v>
@@ -3071,7 +3086,7 @@
     </row>
     <row r="29" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C29" s="18">
         <v>43166</v>
@@ -3165,7 +3180,7 @@
     </row>
     <row r="33" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C33" s="18">
         <v>43179</v>
@@ -3194,7 +3209,7 @@
     </row>
     <row r="34" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C34" s="18">
         <v>43180</v>
@@ -3223,7 +3238,7 @@
     </row>
     <row r="35" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C35" s="18">
         <v>43181</v>
@@ -3252,7 +3267,7 @@
     </row>
     <row r="36" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" s="18">
         <v>43183</v>
@@ -3270,7 +3285,7 @@
     </row>
     <row r="37" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C37" s="18">
         <v>43190</v>
@@ -3279,48 +3294,52 @@
         <v>43190</v>
       </c>
       <c r="E37" s="21">
-        <f t="shared" ref="E37:E43" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
+        <f t="shared" ref="E37:E44" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
         <v>1</v>
       </c>
-      <c r="F37" s="22" t="s">
-        <v>40</v>
+      <c r="F37" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C38" s="18">
-        <v>43193</v>
+        <v>43200</v>
       </c>
       <c r="D38" s="18">
-        <v>43193</v>
+        <v>43200</v>
       </c>
       <c r="E38" s="21">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="F38" s="22" t="s">
-        <v>40</v>
+      <c r="F38" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="21" t="str">
+        <v>43</v>
+      </c>
+      <c r="C39" s="18">
+        <v>43205</v>
+      </c>
+      <c r="D39" s="18">
+        <v>43205</v>
+      </c>
+      <c r="E39" s="21">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F39" s="22" t="s">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
@@ -3334,7 +3353,7 @@
     </row>
     <row r="41" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -3348,7 +3367,7 @@
     </row>
     <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -3362,7 +3381,7 @@
     </row>
     <row r="43" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -3376,21 +3395,35 @@
     </row>
     <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="I31:M31"/>

</xml_diff>

<commit_message>
Updated as of 5/1
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a958261cafb92040/DataScience/Capstone/Products/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TMccw\OneDrive\DataScience\Capstone\Local\Products\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>Start Date</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>Meeting with Advisor #4 (Sudip &amp; Craig in person)</t>
+  </si>
+  <si>
+    <t>Meeting #15</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor #7</t>
   </si>
 </sst>
 </file>
@@ -560,9 +566,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$46</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$49</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -660,24 +666,30 @@
                   <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>Meeting #15</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Meeting with Advisor #7</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="36">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="37">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="38">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="39">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="40">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="41">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -685,10 +697,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$44</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$47</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
                 </c:pt>
@@ -784,6 +796,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>43205</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43220</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,9 +1302,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$46</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$49</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -1387,24 +1402,30 @@
                   <c:v>Meeting with Advisor # 6</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>Meeting #15</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Meeting with Advisor #7</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="36">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="37">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="38">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="39">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="40">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="41">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1412,10 +1433,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$44</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$47</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1513,18 +1534,21 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2258,7 +2282,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>78740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2553,10 +2577,10 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:U53"/>
+  <dimension ref="B1:U56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3294,7 +3318,7 @@
         <v>43190</v>
       </c>
       <c r="E37" s="21">
-        <f t="shared" ref="E37:E44" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
+        <f t="shared" ref="E37:E47" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
         <v>1</v>
       </c>
       <c r="F37" s="20" t="s">
@@ -3339,49 +3363,41 @@
     </row>
     <row r="40" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="21" t="str">
+        <v>52</v>
+      </c>
+      <c r="C40" s="18">
+        <v>43220</v>
+      </c>
+      <c r="D40" s="18">
+        <v>43220</v>
+      </c>
+      <c r="E40" s="21">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="21" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F41" s="22" t="s">
-        <v>40</v>
-      </c>
+      <c r="E41" s="21"/>
+      <c r="F41" s="20"/>
     </row>
     <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="17" t="s">
-        <v>9</v>
-      </c>
+      <c r="B42" s="17"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="21" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F42" s="22" t="s">
-        <v>40</v>
-      </c>
+      <c r="E42" s="21"/>
+      <c r="F42" s="20"/>
     </row>
     <row r="43" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="17" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -3395,7 +3411,7 @@
     </row>
     <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
@@ -3409,21 +3425,63 @@
     </row>
     <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="I31:M31"/>

</xml_diff>

<commit_message>
Updated as of 5/17
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TMccw\OneDrive\DataScience\Capstone\Local\Products\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFAA9873-574F-254A-8D37-389DB2D632CB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15810" windowHeight="6480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>Start Date</t>
   </si>
@@ -185,13 +186,22 @@
     <t>Meeting #15</t>
   </si>
   <si>
-    <t>Meeting with Advisor #7</t>
+    <t>Meeting with Advisor (Pablo) # 3</t>
+  </si>
+  <si>
+    <t>Meeting # 16</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor # 7</t>
+  </si>
+  <si>
+    <t>Meeting # 17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -566,9 +576,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$49</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$53</c:f>
               <c:strCache>
-                <c:ptCount val="42"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -669,27 +679,36 @@
                   <c:v>Meeting #15</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Meeting with Advisor #7</c:v>
+                  <c:v>Meeting # 16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Meeting with Advisor (Pablo) # 3</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>Meeting with Advisor # 7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Meeting # 17</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="40">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="41">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="42">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="43">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="44">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="45">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -697,10 +716,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$47</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$51</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
                 </c:pt>
@@ -799,6 +818,21 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>43220</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43223</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43229</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43235</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43237</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1302,9 +1336,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$49</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$53</c:f>
               <c:strCache>
-                <c:ptCount val="42"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -1405,27 +1439,36 @@
                   <c:v>Meeting #15</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>Meeting with Advisor #7</c:v>
+                  <c:v>Meeting # 16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Meeting with Advisor (Pablo) # 3</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>Meeting with Advisor # 7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Meeting # 17</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="40">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="41">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="42">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="43">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="44">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="45">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1433,10 +1476,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$47</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$51</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1536,19 +1579,31 @@
                 <c:pt idx="32">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="41">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="38">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="43">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2282,7 +2337,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>78740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2573,36 +2628,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:U56"/>
+  <dimension ref="B1:U60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="34.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="15.625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="2.125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27.625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.125" style="3"/>
+    <col min="1" max="1" width="2.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="3"/>
     <col min="10" max="10" width="1.5" style="3" customWidth="1"/>
     <col min="11" max="11" width="4.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.125" style="3"/>
-    <col min="13" max="13" width="15.125" style="3" customWidth="1"/>
-    <col min="14" max="17" width="11.125" style="3"/>
-    <col min="18" max="19" width="10.625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="11.125" style="3"/>
+    <col min="12" max="12" width="11.1640625" style="3"/>
+    <col min="13" max="13" width="15.1640625" style="3" customWidth="1"/>
+    <col min="14" max="17" width="11.1640625" style="3"/>
+    <col min="18" max="19" width="10.6640625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="11.1640625" style="3"/>
     <col min="21" max="21" width="11.5" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="11.125" style="3"/>
+    <col min="22" max="16384" width="11.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
         <v>34</v>
       </c>
@@ -2613,7 +2668,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
         <v>35</v>
       </c>
@@ -2624,14 +2679,14 @@
       <c r="E2" s="12"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
@@ -2642,7 +2697,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -2655,7 +2710,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2677,7 +2732,7 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
@@ -2710,7 +2765,7 @@
       <c r="Q7" s="28"/>
       <c r="R7" s="28"/>
     </row>
-    <row r="8" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
@@ -2729,7 +2784,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
@@ -2748,7 +2803,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
@@ -2767,7 +2822,7 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="s">
         <v>6</v>
       </c>
@@ -2786,7 +2841,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
@@ -2805,7 +2860,7 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
@@ -2824,7 +2879,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="s">
         <v>21</v>
       </c>
@@ -2843,7 +2898,7 @@
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
         <v>16</v>
       </c>
@@ -2862,7 +2917,7 @@
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:21" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
         <v>17</v>
       </c>
@@ -2881,7 +2936,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="s">
         <v>39</v>
       </c>
@@ -2900,7 +2955,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="17" t="s">
         <v>22</v>
       </c>
@@ -2919,7 +2974,7 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17" t="s">
         <v>25</v>
       </c>
@@ -2938,7 +2993,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="17" t="s">
         <v>23</v>
       </c>
@@ -2957,7 +3012,7 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="17" t="s">
         <v>32</v>
       </c>
@@ -2976,7 +3031,7 @@
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="17" t="s">
         <v>26</v>
       </c>
@@ -2995,7 +3050,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="17" t="s">
         <v>24</v>
       </c>
@@ -3014,7 +3069,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="17" t="s">
         <v>28</v>
       </c>
@@ -3033,7 +3088,7 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="17" t="s">
         <v>29</v>
       </c>
@@ -3052,7 +3107,7 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="17" t="s">
         <v>27</v>
       </c>
@@ -3071,7 +3126,7 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="17" t="s">
         <v>51</v>
       </c>
@@ -3090,7 +3145,7 @@
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
         <v>42</v>
       </c>
@@ -3108,7 +3163,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="17" t="s">
         <v>48</v>
       </c>
@@ -3126,7 +3181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="17" t="s">
         <v>30</v>
       </c>
@@ -3144,7 +3199,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="17" t="s">
         <v>31</v>
       </c>
@@ -3173,7 +3228,7 @@
       <c r="Q31" s="27"/>
       <c r="R31" s="7"/>
     </row>
-    <row r="32" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="17" t="s">
         <v>7</v>
       </c>
@@ -3202,7 +3257,7 @@
       <c r="Q32" s="26"/>
       <c r="R32" s="7"/>
     </row>
-    <row r="33" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="17" t="s">
         <v>44</v>
       </c>
@@ -3231,7 +3286,7 @@
       <c r="Q33" s="24"/>
       <c r="R33" s="7"/>
     </row>
-    <row r="34" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="17" t="s">
         <v>45</v>
       </c>
@@ -3260,7 +3315,7 @@
       <c r="Q34" s="24"/>
       <c r="R34" s="7"/>
     </row>
-    <row r="35" spans="2:18" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="17" t="s">
         <v>46</v>
       </c>
@@ -3289,7 +3344,7 @@
       <c r="Q35" s="24"/>
       <c r="R35" s="7"/>
     </row>
-    <row r="36" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="17" t="s">
         <v>49</v>
       </c>
@@ -3307,7 +3362,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="17" t="s">
         <v>47</v>
       </c>
@@ -3318,14 +3373,14 @@
         <v>43190</v>
       </c>
       <c r="E37" s="21">
-        <f t="shared" ref="E37:E47" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
+        <f t="shared" ref="E37:E51" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
         <v>1</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="17" t="s">
         <v>50</v>
       </c>
@@ -3343,7 +3398,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="17" t="s">
         <v>43</v>
       </c>
@@ -3361,7 +3416,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="17" t="s">
         <v>52</v>
       </c>
@@ -3379,109 +3434,183 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="18">
+        <v>43223</v>
+      </c>
+      <c r="D41" s="18">
+        <v>43223</v>
+      </c>
+      <c r="E41" s="21">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B42" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="20"/>
-    </row>
-    <row r="42" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="20"/>
-    </row>
-    <row r="43" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="18">
+        <v>43229</v>
+      </c>
+      <c r="D42" s="18">
+        <v>43229</v>
+      </c>
+      <c r="E42" s="21">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="18">
+        <v>43235</v>
+      </c>
+      <c r="D43" s="18">
+        <v>43235</v>
+      </c>
+      <c r="E43" s="21">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B44" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="18">
+        <v>43237</v>
+      </c>
+      <c r="D44" s="18">
+        <v>43237</v>
+      </c>
+      <c r="E44" s="21">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="20"/>
+    </row>
+    <row r="46" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="20"/>
+    </row>
+    <row r="47" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B47" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="21" t="str">
+      <c r="C47" s="18">
+        <v>43132</v>
+      </c>
+      <c r="D47" s="18">
+        <v>43238</v>
+      </c>
+      <c r="E47" s="21">
+        <f t="shared" si="6"/>
+        <v>107</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="21" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F43" s="22" t="s">
+      <c r="F48" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="21" t="str">
+    <row r="49" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="21" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F44" s="22" t="s">
+      <c r="F49" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="21" t="str">
+    <row r="50" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B50" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="21" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F45" s="22" t="s">
+      <c r="F50" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="21" t="str">
+    <row r="51" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B51" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="21" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F46" s="22" t="s">
+      <c r="F51" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="21" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="17" t="s">
+    <row r="52" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B52" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="17" t="s">
+    <row r="53" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B53" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="55" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="56" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="57" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="59" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="I31:M31"/>

</xml_diff>

<commit_message>
updated as of 5/18
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFAA9873-574F-254A-8D37-389DB2D632CB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1241060-8FF4-6945-8E88-8B8768E7070F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
   <si>
     <t>Start Date</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Meeting # 17</t>
+  </si>
+  <si>
+    <t>Meeting # 18</t>
   </si>
 </sst>
 </file>
@@ -690,6 +693,9 @@
                 <c:pt idx="36">
                   <c:v>Meeting # 17</c:v>
                 </c:pt>
+                <c:pt idx="37">
+                  <c:v>Meeting # 18</c:v>
+                </c:pt>
                 <c:pt idx="39">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
@@ -830,6 +836,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43237</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43238</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>43132</c:v>
@@ -1450,6 +1459,9 @@
                 <c:pt idx="36">
                   <c:v>Meeting # 17</c:v>
                 </c:pt>
+                <c:pt idx="37">
+                  <c:v>Meeting # 18</c:v>
+                </c:pt>
                 <c:pt idx="39">
                   <c:v>Second Paper Draft (B)</c:v>
                 </c:pt>
@@ -1589,6 +1601,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="39">
@@ -2635,7 +2650,7 @@
   <dimension ref="B1:U60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -3507,11 +3522,22 @@
       </c>
     </row>
     <row r="45" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="17"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="20"/>
+      <c r="B45" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="18">
+        <v>43238</v>
+      </c>
+      <c r="D45" s="18">
+        <v>43238</v>
+      </c>
+      <c r="E45" s="21">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F45" s="20" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="46" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="17"/>

</xml_diff>

<commit_message>
Updates as of 5/27
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1241060-8FF4-6945-8E88-8B8768E7070F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6196372F-4F40-FA4C-9DFB-6C9608D8F85B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
   <si>
     <t>Start Date</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Meeting # 18</t>
+  </si>
+  <si>
+    <t>Meeting # 19</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor (Pablo) # 4</t>
   </si>
 </sst>
 </file>
@@ -579,9 +585,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$53</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$55</c:f>
               <c:strCache>
-                <c:ptCount val="46"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -696,25 +702,31 @@
                 <c:pt idx="37">
                   <c:v>Meeting # 18</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>Second Paper Draft (B)</c:v>
+                </c:pt>
                 <c:pt idx="39">
-                  <c:v>Second Paper Draft (B)</c:v>
+                  <c:v>Meeting # 19</c:v>
                 </c:pt>
                 <c:pt idx="40">
+                  <c:v>Meeting with Advisor (Pablo) # 4</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -722,10 +734,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$51</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
                 </c:pt>
@@ -840,8 +852,14 @@
                 <c:pt idx="37">
                   <c:v>43238</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>43132</c:v>
+                </c:pt>
                 <c:pt idx="39">
-                  <c:v>43132</c:v>
+                  <c:v>43247</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1345,9 +1363,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$53</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$55</c:f>
               <c:strCache>
-                <c:ptCount val="46"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -1462,25 +1480,31 @@
                 <c:pt idx="37">
                   <c:v>Meeting # 18</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>Second Paper Draft (B)</c:v>
+                </c:pt>
                 <c:pt idx="39">
-                  <c:v>Second Paper Draft (B)</c:v>
+                  <c:v>Meeting # 19</c:v>
                 </c:pt>
                 <c:pt idx="40">
+                  <c:v>Meeting with Advisor (Pablo) # 4</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>Third Paper Draft (B)</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1488,10 +1512,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$51</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$53</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1606,19 +1630,25 @@
                 <c:pt idx="37">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>107</c:v>
+                </c:pt>
                 <c:pt idx="39">
-                  <c:v>107</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2352,7 +2382,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>78740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2647,10 +2677,10 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:U60"/>
+  <dimension ref="B1:U62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -3388,7 +3418,7 @@
         <v>43190</v>
       </c>
       <c r="E37" s="21">
-        <f t="shared" ref="E37:E51" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
+        <f t="shared" ref="E37:E53" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
         <v>1</v>
       </c>
       <c r="F37" s="20" t="s">
@@ -3540,25 +3570,36 @@
       </c>
     </row>
     <row r="46" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="17"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="20"/>
+      <c r="B46" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="18">
+        <v>43132</v>
+      </c>
+      <c r="D46" s="18">
+        <v>43238</v>
+      </c>
+      <c r="E46" s="21">
+        <f t="shared" si="6"/>
+        <v>107</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="47" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="17" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C47" s="18">
-        <v>43132</v>
+        <v>43247</v>
       </c>
       <c r="D47" s="18">
-        <v>43238</v>
+        <v>43247</v>
       </c>
       <c r="E47" s="21">
-        <f t="shared" si="6"/>
-        <v>107</v>
+        <f t="shared" ref="E47:E48" si="7">IF(ISBLANK(C47),"", (D47-C47+1))</f>
+        <v>1</v>
       </c>
       <c r="F47" s="20" t="s">
         <v>38</v>
@@ -3566,35 +3607,34 @@
     </row>
     <row r="48" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="21" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+        <v>59</v>
+      </c>
+      <c r="C48" s="18">
+        <v>43250</v>
+      </c>
+      <c r="D48" s="18">
+        <v>43250</v>
+      </c>
+      <c r="E48" s="21">
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="F48" s="22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="17" t="s">
-        <v>9</v>
-      </c>
+      <c r="B49" s="17"/>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
-      <c r="E49" s="21" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="E49" s="21"/>
       <c r="F49" s="22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
@@ -3608,7 +3648,7 @@
     </row>
     <row r="51" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
@@ -3622,21 +3662,49 @@
     </row>
     <row r="52" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="17" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B54" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="56" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="57" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="58" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="59" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="60" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="62" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="I31:M31"/>

</xml_diff>

<commit_message>
Updated as of 7/1/18
</commit_message>
<xml_diff>
--- a/Papers/MSDSCapstoneProjectDesignPlan.xlsx
+++ b/Papers/MSDSCapstoneProjectDesignPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmcwilliams/Documents/DataScience/Capstone/Products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6196372F-4F40-FA4C-9DFB-6C9608D8F85B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3A591B-F92D-6245-A8FF-4DFEFC2A254C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Manual Gantt Chart" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
   <si>
     <t>Start Date</t>
   </si>
@@ -51,9 +51,6 @@
     <t>First Paper Draft (A)</t>
   </si>
   <si>
-    <t>Third Paper Draft (B)</t>
-  </si>
-  <si>
     <t>Peer Review (B)</t>
   </si>
   <si>
@@ -99,18 +96,9 @@
     <t>Meeting # 6</t>
   </si>
   <si>
-    <t>Meeting with Advisor # 2</t>
-  </si>
-  <si>
-    <t>Meeting with Advisor # 1</t>
-  </si>
-  <si>
     <t>Meeting # 7</t>
   </si>
   <si>
-    <t>Meeting with Advisor # 3</t>
-  </si>
-  <si>
     <t>Meeting # 8</t>
   </si>
   <si>
@@ -156,9 +144,6 @@
     <t>Meeting #10</t>
   </si>
   <si>
-    <t>Meeting with Advisor # 6</t>
-  </si>
-  <si>
     <t>Online Café Talk (Dan)</t>
   </si>
   <si>
@@ -192,9 +177,6 @@
     <t>Meeting # 16</t>
   </si>
   <si>
-    <t>Meeting with Advisor # 7</t>
-  </si>
-  <si>
     <t>Meeting # 17</t>
   </si>
   <si>
@@ -205,6 +187,51 @@
   </si>
   <si>
     <t>Meeting with Advisor (Pablo) # 4</t>
+  </si>
+  <si>
+    <t>Meeting # 20</t>
+  </si>
+  <si>
+    <t>Meeting with Advisors # 8</t>
+  </si>
+  <si>
+    <t>Meeting with Advisors # 7</t>
+  </si>
+  <si>
+    <t>Meeting with Advisors # 6</t>
+  </si>
+  <si>
+    <t>Meeting with Advisors # 3</t>
+  </si>
+  <si>
+    <t>Meeting with Advisors # 2</t>
+  </si>
+  <si>
+    <t>Meeting with Advisors # 1</t>
+  </si>
+  <si>
+    <t>Meeting # 21</t>
+  </si>
+  <si>
+    <t>Meeting with Advisors # 9</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Meeting with Dr. Engels &amp; Advisors  #10</t>
+  </si>
+  <si>
+    <t>Meeting #22</t>
+  </si>
+  <si>
+    <t>Third Paper Draft - Complete Draft (B)</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Meeting #23</t>
   </si>
 </sst>
 </file>
@@ -312,7 +339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +372,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,7 +459,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -497,6 +530,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -585,9 +621,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$55</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$61</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -622,7 +658,7 @@
                   <c:v>Meeting # 5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Meeting with Advisor # 1</c:v>
+                  <c:v>Meeting with Advisors # 1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Meeting # 6</c:v>
@@ -634,7 +670,7 @@
                   <c:v>Meeting # 7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Meeting with Advisor # 2</c:v>
+                  <c:v>Meeting with Advisors # 2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Meeting # 8</c:v>
@@ -643,7 +679,7 @@
                   <c:v>Meeting # 9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Meeting with Advisor # 3</c:v>
+                  <c:v>Meeting with Advisors # 3</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>Meeting with Advisor #4 (Sudip &amp; Craig in person)</c:v>
@@ -682,7 +718,7 @@
                   <c:v>Meeting with Advisor (Pablo) # 2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Meeting with Advisor # 6</c:v>
+                  <c:v>Meeting with Advisors # 6</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>Meeting #15</c:v>
@@ -694,7 +730,7 @@
                   <c:v>Meeting with Advisor (Pablo) # 3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Meeting with Advisor # 7</c:v>
+                  <c:v>Meeting with Advisors # 7</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>Meeting # 17</c:v>
@@ -711,22 +747,43 @@
                 <c:pt idx="40">
                   <c:v>Meeting with Advisor (Pablo) # 4</c:v>
                 </c:pt>
+                <c:pt idx="41">
+                  <c:v>Meeting # 20</c:v>
+                </c:pt>
                 <c:pt idx="42">
-                  <c:v>Third Paper Draft (B)</c:v>
+                  <c:v>Meeting with Advisors # 8</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>Meeting # 21</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Meeting with Advisors # 9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Meeting with Dr. Engels &amp; Advisors  #10</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Meeting #22</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Meeting #23</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Third Paper Draft - Complete Draft (B)</c:v>
+                </c:pt>
+                <c:pt idx="49">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="50">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="51">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="52">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="53">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -734,10 +791,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$53</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$C$8:$C$57</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>43118</c:v>
                 </c:pt>
@@ -860,6 +917,30 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>43250</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43258</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43271</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43282</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,9 +1444,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$55</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$B$8:$B$61</c:f>
               <c:strCache>
-                <c:ptCount val="48"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
                   <c:v>Project Kickoff</c:v>
                 </c:pt>
@@ -1400,7 +1481,7 @@
                   <c:v>Meeting # 5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Meeting with Advisor # 1</c:v>
+                  <c:v>Meeting with Advisors # 1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Meeting # 6</c:v>
@@ -1412,7 +1493,7 @@
                   <c:v>Meeting # 7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Meeting with Advisor # 2</c:v>
+                  <c:v>Meeting with Advisors # 2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Meeting # 8</c:v>
@@ -1421,7 +1502,7 @@
                   <c:v>Meeting # 9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>Meeting with Advisor # 3</c:v>
+                  <c:v>Meeting with Advisors # 3</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>Meeting with Advisor #4 (Sudip &amp; Craig in person)</c:v>
@@ -1460,7 +1541,7 @@
                   <c:v>Meeting with Advisor (Pablo) # 2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Meeting with Advisor # 6</c:v>
+                  <c:v>Meeting with Advisors # 6</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>Meeting #15</c:v>
@@ -1472,7 +1553,7 @@
                   <c:v>Meeting with Advisor (Pablo) # 3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>Meeting with Advisor # 7</c:v>
+                  <c:v>Meeting with Advisors # 7</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>Meeting # 17</c:v>
@@ -1489,22 +1570,43 @@
                 <c:pt idx="40">
                   <c:v>Meeting with Advisor (Pablo) # 4</c:v>
                 </c:pt>
+                <c:pt idx="41">
+                  <c:v>Meeting # 20</c:v>
+                </c:pt>
                 <c:pt idx="42">
-                  <c:v>Third Paper Draft (B)</c:v>
+                  <c:v>Meeting with Advisors # 8</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>Meeting # 21</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Meeting with Advisors # 9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Meeting with Dr. Engels &amp; Advisors  #10</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Meeting #22</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Meeting #23</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Third Paper Draft - Complete Draft (B)</c:v>
+                </c:pt>
+                <c:pt idx="49">
                   <c:v>Peer Review (B)</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="50">
                   <c:v>Final Papers (B)</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="51">
                   <c:v>Poster Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="52">
                   <c:v>Lightning Presentation (B)</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="53">
                   <c:v>Final Paper/Publication</c:v>
                 </c:pt>
               </c:strCache>
@@ -1512,10 +1614,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$53</c:f>
+              <c:f>'Basic Manual Gantt Chart'!$E$8:$E$57</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1639,16 +1741,31 @@
                 <c:pt idx="40">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="49">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2382,7 +2499,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>78740</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2677,10 +2794,10 @@
   <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:U62"/>
+  <dimension ref="B1:U66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2704,10 +2821,10 @@
   <sheetData>
     <row r="1" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -2715,10 +2832,10 @@
     </row>
     <row r="2" spans="2:21" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -2750,7 +2867,7 @@
         <v>43332</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
@@ -2791,7 +2908,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="2" t="s">
@@ -2825,13 +2942,13 @@
         <v>1</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="18">
         <v>43118</v>
@@ -2844,13 +2961,13 @@
         <v>1</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="18">
         <v>43118</v>
@@ -2863,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -2882,13 +2999,13 @@
         <v>14</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="18">
         <v>43124</v>
@@ -2901,13 +3018,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="18">
         <v>43124</v>
@@ -2920,13 +3037,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="18">
         <v>43124</v>
@@ -2939,13 +3056,13 @@
         <v>8</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="18">
         <v>43129</v>
@@ -2958,13 +3075,13 @@
         <v>1</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="2:21" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="18">
         <v>43130</v>
@@ -2977,13 +3094,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C17" s="18">
         <v>43131</v>
@@ -2996,13 +3113,13 @@
         <v>1</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="18">
         <v>43132</v>
@@ -3015,13 +3132,13 @@
         <v>1</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C19" s="18">
         <v>43132</v>
@@ -3034,13 +3151,13 @@
         <v>1</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="18">
         <v>43135</v>
@@ -3053,13 +3170,13 @@
         <v>1</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C21" s="18">
         <v>43138</v>
@@ -3072,13 +3189,13 @@
         <v>2</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C22" s="18">
         <v>43141</v>
@@ -3091,13 +3208,13 @@
         <v>1</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="17" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="C23" s="18">
         <v>43144</v>
@@ -3110,13 +3227,13 @@
         <v>1</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C24" s="18">
         <v>43148</v>
@@ -3129,13 +3246,13 @@
         <v>1</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C25" s="18">
         <v>43156</v>
@@ -3148,13 +3265,13 @@
         <v>1</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="17" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C26" s="18">
         <v>43162</v>
@@ -3167,13 +3284,13 @@
         <v>1</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="17" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C27" s="18">
         <v>43165</v>
@@ -3186,13 +3303,13 @@
         <v>1</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C28" s="18">
         <v>43165</v>
@@ -3205,12 +3322,12 @@
         <v>1</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C29" s="18">
         <v>43166</v>
@@ -3223,12 +3340,12 @@
         <v>1</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C30" s="18">
         <v>43170</v>
@@ -3241,12 +3358,12 @@
         <v>1</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C31" s="18">
         <v>43173</v>
@@ -3259,7 +3376,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="25"/>
@@ -3288,7 +3405,7 @@
         <v>42</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="26"/>
@@ -3304,7 +3421,7 @@
     </row>
     <row r="33" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C33" s="18">
         <v>43179</v>
@@ -3317,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="24"/>
@@ -3333,7 +3450,7 @@
     </row>
     <row r="34" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C34" s="18">
         <v>43180</v>
@@ -3346,7 +3463,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="24"/>
@@ -3362,7 +3479,7 @@
     </row>
     <row r="35" spans="2:18" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C35" s="18">
         <v>43181</v>
@@ -3375,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="24"/>
@@ -3391,7 +3508,7 @@
     </row>
     <row r="36" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C36" s="18">
         <v>43183</v>
@@ -3404,12 +3521,12 @@
         <v>1</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C37" s="18">
         <v>43190</v>
@@ -3418,16 +3535,16 @@
         <v>43190</v>
       </c>
       <c r="E37" s="21">
-        <f t="shared" ref="E37:E53" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
+        <f t="shared" ref="E37:E57" si="6">IF(ISBLANK(C37),"", (D37-C37+1))</f>
         <v>1</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C38" s="18">
         <v>43200</v>
@@ -3440,12 +3557,12 @@
         <v>1</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="17" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C39" s="18">
         <v>43205</v>
@@ -3458,12 +3575,12 @@
         <v>1</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C40" s="18">
         <v>43220</v>
@@ -3476,12 +3593,12 @@
         <v>1</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C41" s="18">
         <v>43223</v>
@@ -3494,12 +3611,12 @@
         <v>1</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C42" s="18">
         <v>43229</v>
@@ -3512,12 +3629,12 @@
         <v>1</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C43" s="18">
         <v>43235</v>
@@ -3530,12 +3647,12 @@
         <v>1</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="17" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C44" s="18">
         <v>43237</v>
@@ -3548,12 +3665,12 @@
         <v>1</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C45" s="18">
         <v>43238</v>
@@ -3566,12 +3683,12 @@
         <v>1</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C46" s="18">
         <v>43132</v>
@@ -3584,12 +3701,12 @@
         <v>107</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C47" s="18">
         <v>43247</v>
@@ -3598,16 +3715,16 @@
         <v>43247</v>
       </c>
       <c r="E47" s="21">
-        <f t="shared" ref="E47:E48" si="7">IF(ISBLANK(C47),"", (D47-C47+1))</f>
+        <f t="shared" ref="E47:E53" si="7">IF(ISBLANK(C47),"", (D47-C47+1))</f>
         <v>1</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C48" s="18">
         <v>43250</v>
@@ -3619,92 +3736,233 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="F48" s="22" t="s">
-        <v>40</v>
+      <c r="F48" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="22" t="s">
-        <v>40</v>
+      <c r="B49" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="18">
+        <v>43258</v>
+      </c>
+      <c r="D49" s="18">
+        <v>43258</v>
+      </c>
+      <c r="E49" s="21">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="18">
+        <v>43271</v>
+      </c>
+      <c r="D50" s="18">
+        <v>43271</v>
+      </c>
+      <c r="E50" s="21">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B51" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="18">
+        <v>43282</v>
+      </c>
+      <c r="D51" s="18">
+        <v>43282</v>
+      </c>
+      <c r="E51" s="21">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B52" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52" s="21" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B53" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53" s="21" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B54" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E54" s="21" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" s="21" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B56" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="18">
+        <v>43132</v>
+      </c>
+      <c r="D56" s="18">
+        <v>43292</v>
+      </c>
+      <c r="E56" s="21">
+        <f t="shared" si="6"/>
+        <v>161</v>
+      </c>
+      <c r="F56" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B57" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="21" t="str">
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="21" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F50" s="22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="17" t="s">
+      <c r="F57" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B58" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="21" t="str">
-        <f t="shared" si="6"/>
+      <c r="C58" s="18">
+        <v>43132</v>
+      </c>
+      <c r="D58" s="18">
+        <v>43329</v>
+      </c>
+      <c r="E58" s="21">
+        <f t="shared" ref="E58:E61" si="8">IF(ISBLANK(C58),"", (D58-C58+1))</f>
+        <v>198</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B59" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="21" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="F51" s="22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B52" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="21" t="str">
-        <f t="shared" si="6"/>
+      <c r="F59" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B60" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="21" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="F52" s="22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B53" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="21" t="str">
-        <f t="shared" si="6"/>
+      <c r="F60" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B61" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="21" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="F53" s="22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B54" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B55" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="57" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="60" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="F61" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="62" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="I31:M31"/>

</xml_diff>